<commit_message>
changed pip version because Pacmap (-> not running perfectly), built prototype for correlation, clustering, classification, general_statistics, added feature_preprocessing_table.xlsx, finished cache_IO.py
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EB3E0A-B924-4D71-87CA-02133AC7017B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5F9F6C-7EA2-4ACE-9663-3E4B106EF3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3228" windowWidth="23040" windowHeight="12120" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="102">
   <si>
     <t>row_id</t>
   </si>
@@ -310,12 +310,6 @@
     <t>comment</t>
   </si>
   <si>
-    <t>missing_rate</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>vitals</t>
   </si>
   <si>
@@ -346,9 +340,6 @@
     <t>can also be used to categorize patients with</t>
   </si>
   <si>
-    <t>very important to seperate stroke-types</t>
-  </si>
-  <si>
     <t>was used to seperate stroke_type</t>
   </si>
   <si>
@@ -367,25 +358,49 @@
     <t>none</t>
   </si>
   <si>
-    <t>categorical, once</t>
-  </si>
-  <si>
-    <t>categorical, binary</t>
-  </si>
-  <si>
-    <t>categorical, once, binary</t>
-  </si>
-  <si>
-    <t>categorical, once (multiple)</t>
-  </si>
-  <si>
     <t>continuous</t>
   </si>
   <si>
-    <t>continuous, once</t>
-  </si>
-  <si>
     <t>categorical_or_continuous</t>
+  </si>
+  <si>
+    <t>single_value</t>
+  </si>
+  <si>
+    <t>flag_value</t>
+  </si>
+  <si>
+    <t>potential_for_analysis</t>
+  </si>
+  <si>
+    <t>maybe</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>must be included</t>
+  </si>
+  <si>
+    <t>must be included to seperate stroke-types</t>
+  </si>
+  <si>
+    <t>prediction variable is selected inside Python</t>
+  </si>
+  <si>
+    <t>needs_binning</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>international normalized ratio</t>
+  </si>
+  <si>
+    <t>not_for_classification</t>
   </si>
 </sst>
 </file>
@@ -751,7 +766,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -759,1041 +774,1251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49:D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
-    <col min="4" max="4" width="35.109375" customWidth="1"/>
+    <col min="3" max="4" width="35.109375" customWidth="1"/>
     <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" customWidth="1"/>
+    <col min="7" max="7" width="49.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="G6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>76</v>
       </c>
       <c r="F7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="G7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C15" t="s">
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="G15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C21" t="s">
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C24" t="s">
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C26" t="s">
+        <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
         <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="G27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="E28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="F28" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
+        <v>72</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>72</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>72</v>
       </c>
       <c r="D33" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>87</v>
+      </c>
+      <c r="C34" t="s">
+        <v>72</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="E34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>72</v>
       </c>
       <c r="D35" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="E35" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>73</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C37" t="s">
+        <v>73</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>73</v>
       </c>
       <c r="D38" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
+        <v>73</v>
       </c>
       <c r="D39" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="E39" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
       </c>
       <c r="D40" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="E40" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>72</v>
       </c>
       <c r="D41" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="E41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>73</v>
       </c>
       <c r="D42" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="E42" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="C43" t="s">
+        <v>73</v>
       </c>
       <c r="D43" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="E43" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>73</v>
       </c>
       <c r="D44" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="E44" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>73</v>
       </c>
       <c r="D45" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="E45" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>74</v>
       </c>
       <c r="D46" t="s">
-        <v>76</v>
-      </c>
-      <c r="F46" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="E46" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
       <c r="B47" t="s">
         <v>89</v>
       </c>
-      <c r="C47">
-        <v>0</v>
+      <c r="C47" t="s">
+        <v>73</v>
       </c>
       <c r="D47" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>89</v>
       </c>
-      <c r="C48">
-        <v>0</v>
+      <c r="C48" t="s">
+        <v>75</v>
       </c>
       <c r="D48" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>92</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="C49" t="s">
+        <v>75</v>
       </c>
       <c r="D49" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="E49" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
-      </c>
-      <c r="C50">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="C50" t="s">
+        <v>75</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="E50" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="C51" t="s">
+        <v>75</v>
       </c>
       <c r="D51" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="E51" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="C52" t="s">
+        <v>75</v>
       </c>
       <c r="D52" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="E52" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
-      </c>
-      <c r="C53">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="C53" t="s">
+        <v>75</v>
       </c>
       <c r="D53" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="E53" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="C54" t="s">
+        <v>74</v>
       </c>
       <c r="D54" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="E54" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="C55" t="s">
+        <v>74</v>
       </c>
       <c r="D55" t="s">
-        <v>76</v>
-      </c>
-      <c r="F55" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="E55" t="s">
+        <v>92</v>
+      </c>
+      <c r="G55" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>90</v>
-      </c>
-      <c r="C56">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="C56" t="s">
+        <v>72</v>
       </c>
       <c r="D56" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="E56" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="C57" t="s">
+        <v>74</v>
       </c>
       <c r="D57" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="E57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>91</v>
-      </c>
-      <c r="C58">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="C58" t="s">
+        <v>74</v>
       </c>
       <c r="D58" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="E58" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>92</v>
-      </c>
-      <c r="C59">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="C59" t="s">
+        <v>74</v>
       </c>
       <c r="D59" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="E59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>90</v>
-      </c>
-      <c r="C60">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="C60" t="s">
+        <v>74</v>
       </c>
       <c r="D60" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="E60" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F60" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="G60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>92</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="C61" t="s">
+        <v>74</v>
       </c>
       <c r="D61" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="E61" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>92</v>
-      </c>
-      <c r="C62">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="C62" t="s">
+        <v>74</v>
       </c>
       <c r="D62" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="E62" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
-      </c>
-      <c r="C63">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="C63" t="s">
+        <v>74</v>
       </c>
       <c r="D63" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="E63" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F63" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>92</v>
-      </c>
-      <c r="C64">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="C64" t="s">
+        <v>74</v>
       </c>
       <c r="D64" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="E64" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
-      </c>
-      <c r="C65">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="C65" t="s">
+        <v>74</v>
       </c>
       <c r="D65" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="E65" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
-      </c>
-      <c r="C66">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="C66" t="s">
+        <v>74</v>
       </c>
       <c r="D66" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="E66" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F66" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>90</v>
-      </c>
-      <c r="C67">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="C67" t="s">
+        <v>74</v>
       </c>
       <c r="D67" t="s">
-        <v>76</v>
-      </c>
-      <c r="F67" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="G67" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>93</v>
-      </c>
-      <c r="C68">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="C68" t="s">
+        <v>74</v>
       </c>
       <c r="D68" t="s">
-        <v>76</v>
-      </c>
-      <c r="F68" t="s">
-        <v>80</v>
+        <v>101</v>
+      </c>
+      <c r="G68" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small additions to clustering, general_statistics
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5F9F6C-7EA2-4ACE-9663-3E4B106EF3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B6A46F-299D-4CC9-BCAF-C554FB1BBF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
+    <workbookView xWindow="4080" yWindow="3924" windowWidth="23040" windowHeight="12120" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="102">
   <si>
     <t>row_id</t>
   </si>
@@ -776,17 +776,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49:D53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="4" width="35.109375" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" customWidth="1"/>
     <col min="7" max="7" width="49.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -846,9 +847,6 @@
       <c r="E3" t="s">
         <v>76</v>
       </c>
-      <c r="F3" t="s">
-        <v>76</v>
-      </c>
       <c r="G3" t="s">
         <v>84</v>
       </c>
@@ -886,9 +884,6 @@
       <c r="E5" t="s">
         <v>76</v>
       </c>
-      <c r="F5" t="s">
-        <v>76</v>
-      </c>
       <c r="G5" t="s">
         <v>82</v>
       </c>
@@ -992,9 +987,6 @@
       <c r="E10" t="s">
         <v>76</v>
       </c>
-      <c r="F10" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1046,9 +1038,6 @@
       <c r="E13" t="s">
         <v>76</v>
       </c>
-      <c r="F13" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1171,9 +1160,6 @@
       <c r="E20" t="s">
         <v>76</v>
       </c>
-      <c r="F20" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -1443,9 +1429,6 @@
       <c r="E36" t="s">
         <v>76</v>
       </c>
-      <c r="F36" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -1463,9 +1446,6 @@
       <c r="E37" t="s">
         <v>76</v>
       </c>
-      <c r="F37" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -1483,9 +1463,6 @@
       <c r="E38" t="s">
         <v>76</v>
       </c>
-      <c r="F38" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -1503,9 +1480,6 @@
       <c r="E39" t="s">
         <v>76</v>
       </c>
-      <c r="F39" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -1557,9 +1531,6 @@
       <c r="E42" t="s">
         <v>76</v>
       </c>
-      <c r="F42" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
@@ -1929,9 +1900,6 @@
       <c r="E63" t="s">
         <v>76</v>
       </c>
-      <c r="F63" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
@@ -1981,9 +1949,6 @@
         <v>99</v>
       </c>
       <c r="E66" t="s">
-        <v>76</v>
-      </c>
-      <c r="F66" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added NAN Count to calculate_feature_overview_table, also sorted table
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B6A46F-299D-4CC9-BCAF-C554FB1BBF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913A38BE-0D0B-4C39-A017-79F3D4130D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="3924" windowWidth="23040" windowHeight="12120" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="102">
   <si>
     <t>row_id</t>
   </si>
@@ -766,7 +766,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1429,6 +1429,9 @@
       <c r="E36" t="s">
         <v>76</v>
       </c>
+      <c r="F36" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -1446,6 +1449,9 @@
       <c r="E37" t="s">
         <v>76</v>
       </c>
+      <c r="F37" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -1461,6 +1467,9 @@
         <v>99</v>
       </c>
       <c r="E38" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished feature_selection for import of carevue+metavision patients, added use_case_name to output folder
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913A38BE-0D0B-4C39-A017-79F3D4130D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52D0853-7137-4510-BE6F-4D9663EB75A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="103">
   <si>
     <t>row_id</t>
   </si>
@@ -139,15 +139,6 @@
     <t>INR</t>
   </si>
   <si>
-    <t>Non Invasive Blood Pressure diastolic</t>
-  </si>
-  <si>
-    <t>Non Invasive Blood Pressure mean</t>
-  </si>
-  <si>
-    <t>Non Invasive Blood Pressure systolic</t>
-  </si>
-  <si>
     <t>O2 saturation pulseoxymetry</t>
   </si>
   <si>
@@ -401,6 +392,18 @@
   </si>
   <si>
     <t>not_for_classification</t>
+  </si>
+  <si>
+    <t>infarct_type</t>
+  </si>
+  <si>
+    <t>must be included to seperate infarct-types</t>
+  </si>
+  <si>
+    <t>dbsource</t>
+  </si>
+  <si>
+    <t>metavision or carevue</t>
   </si>
 </sst>
 </file>
@@ -774,10 +777,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,32 +790,32 @@
     <col min="2" max="2" width="23.88671875" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" customWidth="1"/>
     <col min="7" max="7" width="49.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -819,16 +823,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -836,19 +840,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -856,16 +860,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -873,19 +877,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -893,22 +897,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -916,22 +920,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -939,19 +943,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -959,16 +963,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -976,16 +980,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -993,16 +997,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1010,16 +1014,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1027,16 +1031,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1044,16 +1048,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1061,19 +1065,19 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1081,16 +1085,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1098,16 +1102,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1115,16 +1119,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1132,16 +1136,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1149,16 +1153,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1166,16 +1170,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1183,16 +1187,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1200,16 +1204,19 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="F23" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1217,16 +1224,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
         <v>98</v>
       </c>
-      <c r="E24" t="s">
-        <v>76</v>
+      <c r="G24" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1234,16 +1241,22 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
         <v>98</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>90</v>
+      </c>
+      <c r="F25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1251,19 +1264,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
         <v>98</v>
-      </c>
-      <c r="E26" t="s">
-        <v>76</v>
-      </c>
-      <c r="F26" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1274,13 +1281,10 @@
         <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s">
-        <v>101</v>
-      </c>
-      <c r="G27" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1288,22 +1292,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
-      </c>
-      <c r="E28" t="s">
-        <v>93</v>
-      </c>
-      <c r="F28" t="s">
-        <v>76</v>
-      </c>
-      <c r="G28" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1311,13 +1306,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1325,674 +1320,678 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="E30" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="E31" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" t="s">
         <v>89</v>
-      </c>
-      <c r="C32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E33" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E34" t="s">
-        <v>92</v>
+        <v>73</v>
+      </c>
+      <c r="F34" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D35" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E35" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="F35" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E36" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F36" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>76</v>
-      </c>
-      <c r="F37" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E38" t="s">
-        <v>76</v>
-      </c>
-      <c r="F38" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D39" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E39" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E40" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D41" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C42" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D42" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E42" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D43" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E43" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" t="s">
+        <v>71</v>
+      </c>
+      <c r="D44" t="s">
+        <v>98</v>
+      </c>
+      <c r="E44" t="s">
         <v>89</v>
       </c>
-      <c r="C44" t="s">
-        <v>73</v>
-      </c>
-      <c r="D44" t="s">
-        <v>99</v>
-      </c>
-      <c r="E44" t="s">
-        <v>76</v>
+      <c r="G44" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C45" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>99</v>
-      </c>
-      <c r="E45" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D46" t="s">
-        <v>101</v>
-      </c>
-      <c r="E46" t="s">
-        <v>92</v>
-      </c>
-      <c r="G46" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D47" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="E47" t="s">
+        <v>76</v>
+      </c>
+      <c r="G47" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C48" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D48" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="E48" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D49" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E49" t="s">
-        <v>79</v>
-      </c>
-      <c r="G49" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C50" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D50" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E50" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C51" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D51" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E51" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C52" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D52" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E52" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" t="s">
+        <v>95</v>
+      </c>
+      <c r="E53" t="s">
         <v>89</v>
       </c>
-      <c r="C53" t="s">
-        <v>75</v>
-      </c>
-      <c r="D53" t="s">
-        <v>99</v>
-      </c>
-      <c r="E53" t="s">
-        <v>79</v>
+      <c r="G53" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D54" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C55" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D55" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E55" t="s">
-        <v>92</v>
-      </c>
-      <c r="G55" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D56" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E56" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="F56" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
         <v>87</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D57" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E57" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C58" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D58" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E58" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F58" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="G58" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D59" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E59" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="F59" t="s">
+        <v>73</v>
+      </c>
+      <c r="G59" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C60" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D60" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E60" t="s">
-        <v>83</v>
-      </c>
-      <c r="F60" t="s">
-        <v>76</v>
-      </c>
-      <c r="G60" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C61" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D61" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E61" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D62" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E62" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B63" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D63" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E63" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C64" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D64" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E64" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C65" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D65" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E65" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C66" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D66" t="s">
-        <v>99</v>
-      </c>
-      <c r="E66" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="G66" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D67" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G67" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>66</v>
-      </c>
-      <c r="B68" t="s">
-        <v>89</v>
-      </c>
-      <c r="C68" t="s">
-        <v>74</v>
-      </c>
-      <c r="D68" t="s">
-        <v>101</v>
-      </c>
-      <c r="G68" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added use_case_name to outputs
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52D0853-7137-4510-BE6F-4D9663EB75A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FE7B86-CD3C-47AC-8B82-7C4AEE984D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="103">
   <si>
     <t>row_id</t>
   </si>
@@ -780,8 +780,8 @@
   <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -851,6 +851,9 @@
       <c r="E3" t="s">
         <v>73</v>
       </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
       <c r="G3" t="s">
         <v>81</v>
       </c>
@@ -931,9 +934,6 @@
       <c r="E7" t="s">
         <v>73</v>
       </c>
-      <c r="F7" t="s">
-        <v>73</v>
-      </c>
       <c r="G7" t="s">
         <v>79</v>
       </c>
@@ -974,6 +974,9 @@
       <c r="E9" t="s">
         <v>73</v>
       </c>
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -991,6 +994,9 @@
       <c r="E10" t="s">
         <v>73</v>
       </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1008,6 +1014,9 @@
       <c r="E11" t="s">
         <v>73</v>
       </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1025,6 +1034,9 @@
       <c r="E12" t="s">
         <v>73</v>
       </c>
+      <c r="F12" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1042,6 +1054,9 @@
       <c r="E13" t="s">
         <v>73</v>
       </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1059,6 +1074,9 @@
       <c r="E14" t="s">
         <v>73</v>
       </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1076,6 +1094,9 @@
       <c r="E15" t="s">
         <v>73</v>
       </c>
+      <c r="F15" t="s">
+        <v>73</v>
+      </c>
       <c r="G15" t="s">
         <v>97</v>
       </c>
@@ -1096,6 +1117,9 @@
       <c r="E16" t="s">
         <v>73</v>
       </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -1113,6 +1137,9 @@
       <c r="E17" t="s">
         <v>73</v>
       </c>
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -1130,6 +1157,9 @@
       <c r="E18" t="s">
         <v>73</v>
       </c>
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -1147,6 +1177,9 @@
       <c r="E19" t="s">
         <v>73</v>
       </c>
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -1164,6 +1197,9 @@
       <c r="E20" t="s">
         <v>73</v>
       </c>
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -1181,6 +1217,9 @@
       <c r="E21" t="s">
         <v>73</v>
       </c>
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -1198,6 +1237,9 @@
       <c r="E22" t="s">
         <v>73</v>
       </c>
+      <c r="F22" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -1465,6 +1507,9 @@
       <c r="E37" t="s">
         <v>73</v>
       </c>
+      <c r="F37" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -1516,6 +1561,9 @@
       <c r="E40" t="s">
         <v>73</v>
       </c>
+      <c r="F40" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
@@ -1720,6 +1768,9 @@
       <c r="E52" t="s">
         <v>73</v>
       </c>
+      <c r="F52" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
@@ -1874,6 +1925,9 @@
       <c r="E60" t="s">
         <v>73</v>
       </c>
+      <c r="F60" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
@@ -1891,6 +1945,9 @@
       <c r="E61" t="s">
         <v>73</v>
       </c>
+      <c r="F61" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
@@ -1908,6 +1965,9 @@
       <c r="E62" t="s">
         <v>73</v>
       </c>
+      <c r="F62" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -1925,6 +1985,9 @@
       <c r="E63" t="s">
         <v>73</v>
       </c>
+      <c r="F63" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
@@ -1942,6 +2005,9 @@
       <c r="E64" t="s">
         <v>73</v>
       </c>
+      <c r="F64" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
@@ -1957,6 +2023,9 @@
         <v>96</v>
       </c>
       <c r="E65" t="s">
+        <v>73</v>
+      </c>
+      <c r="F65" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added outlier removal, now clean clusters, added standardization, now recall at 0.28
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FE7B86-CD3C-47AC-8B82-7C4AEE984D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F35ED7B-1713-4269-A465-5CBC981F3FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="103">
   <si>
     <t>row_id</t>
   </si>
@@ -780,8 +780,8 @@
   <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,9 +974,6 @@
       <c r="E9" t="s">
         <v>73</v>
       </c>
-      <c r="F9" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -994,9 +991,6 @@
       <c r="E10" t="s">
         <v>73</v>
       </c>
-      <c r="F10" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1014,9 +1008,6 @@
       <c r="E11" t="s">
         <v>73</v>
       </c>
-      <c r="F11" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1034,9 +1025,6 @@
       <c r="E12" t="s">
         <v>73</v>
       </c>
-      <c r="F12" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1054,9 +1042,6 @@
       <c r="E13" t="s">
         <v>73</v>
       </c>
-      <c r="F13" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1074,9 +1059,6 @@
       <c r="E14" t="s">
         <v>73</v>
       </c>
-      <c r="F14" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1157,9 +1139,6 @@
       <c r="E18" t="s">
         <v>73</v>
       </c>
-      <c r="F18" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -1177,9 +1156,6 @@
       <c r="E19" t="s">
         <v>73</v>
       </c>
-      <c r="F19" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -1197,9 +1173,6 @@
       <c r="E20" t="s">
         <v>73</v>
       </c>
-      <c r="F20" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -1217,9 +1190,6 @@
       <c r="E21" t="s">
         <v>73</v>
       </c>
-      <c r="F21" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -1237,9 +1207,6 @@
       <c r="E22" t="s">
         <v>73</v>
       </c>
-      <c r="F22" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -1467,9 +1434,6 @@
       <c r="E35" t="s">
         <v>73</v>
       </c>
-      <c r="F35" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -1507,9 +1471,6 @@
       <c r="E37" t="s">
         <v>73</v>
       </c>
-      <c r="F37" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -1925,9 +1886,6 @@
       <c r="E60" t="s">
         <v>73</v>
       </c>
-      <c r="F60" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
@@ -1945,9 +1903,6 @@
       <c r="E61" t="s">
         <v>73</v>
       </c>
-      <c r="F61" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
@@ -1965,9 +1920,6 @@
       <c r="E62" t="s">
         <v>73</v>
       </c>
-      <c r="F62" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -1985,9 +1937,6 @@
       <c r="E63" t="s">
         <v>73</v>
       </c>
-      <c r="F63" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
@@ -2005,9 +1954,6 @@
       <c r="E64" t="s">
         <v>73</v>
       </c>
-      <c r="F64" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
@@ -2023,9 +1969,6 @@
         <v>96</v>
       </c>
       <c r="E65" t="s">
-        <v>73</v>
-      </c>
-      <c r="F65" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
moved preprocessing outside of functions, added clusters and dynamic features to features_overview_clusters, for this also added supplements/factorization_table.csv
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F35ED7B-1713-4269-A465-5CBC981F3FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19626651-D2EE-42F8-9A67-2D2056A934D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="106">
   <si>
     <t>row_id</t>
   </si>
@@ -319,30 +319,15 @@
     <t>yes</t>
   </si>
   <si>
-    <t>not in analysis, first use avgs, later per hour</t>
-  </si>
-  <si>
     <t>not in analysis, but might interesting for secondary illnesses</t>
   </si>
   <si>
-    <t>prediction variable</t>
-  </si>
-  <si>
     <t>can also be used to categorize patients with</t>
   </si>
   <si>
     <t>was used to seperate stroke_type</t>
   </si>
   <si>
-    <t>might be important, for now only 'non invasive bp'</t>
-  </si>
-  <si>
-    <t>no, but must be used as filter</t>
-  </si>
-  <si>
-    <t>might also be useful if categorical?</t>
-  </si>
-  <si>
     <t>ids for pandas dataframes</t>
   </si>
   <si>
@@ -367,12 +352,6 @@
     <t>maybe</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>must be included</t>
-  </si>
-  <si>
     <t>must be included to seperate stroke-types</t>
   </si>
   <si>
@@ -403,7 +382,37 @@
     <t>dbsource</t>
   </si>
   <si>
-    <t>metavision or carevue</t>
+    <t>must_be_removed</t>
+  </si>
+  <si>
+    <t>must be included for filter</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>must be included for id</t>
+  </si>
+  <si>
+    <t>metavision or carevue, only used for filtering</t>
+  </si>
+  <si>
+    <t>categorical</t>
+  </si>
+  <si>
+    <t>datetime not useful</t>
+  </si>
+  <si>
+    <t>transformation to in does not work, preiculos is 'string' in format day:hour:minute, this feature is not that important</t>
+  </si>
+  <si>
+    <t>prediction_variable</t>
+  </si>
+  <si>
+    <t>not in analysis because too many categories, but might interesting</t>
+  </si>
+  <si>
+    <t>not remove because needed in clustering, but remove in python for correlation &amp; classification</t>
   </si>
 </sst>
 </file>
@@ -777,11 +786,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,61 +801,71 @@
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="27.5546875" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" customWidth="1"/>
-    <col min="7" max="7" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="39.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
         <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="H2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
         <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
         <v>73</v>
@@ -854,59 +873,59 @@
       <c r="F3" t="s">
         <v>73</v>
       </c>
-      <c r="G3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
         <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
         <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
         <v>73</v>
       </c>
-      <c r="G5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
         <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E6" t="s">
         <v>73</v>
@@ -914,42 +933,39 @@
       <c r="F6" t="s">
         <v>73</v>
       </c>
-      <c r="G6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
         <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E7" t="s">
         <v>73</v>
       </c>
-      <c r="G7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
         <v>73</v>
@@ -958,120 +974,138 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
         <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E9" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
         <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
         <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
         <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
         <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E13" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
         <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
         <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E15" t="s">
         <v>73</v>
@@ -1079,22 +1113,22 @@
       <c r="F15" t="s">
         <v>73</v>
       </c>
-      <c r="G15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
         <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E16" t="s">
         <v>73</v>
@@ -1103,18 +1137,18 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
         <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E17" t="s">
         <v>73</v>
@@ -1123,103 +1157,118 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
         <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E18" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
         <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
         <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E20" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E21" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
         <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E22" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
         <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E23" t="s">
         <v>73</v>
@@ -1228,188 +1277,263 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
         <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>91</v>
+      </c>
+      <c r="E24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" t="s">
+        <v>73</v>
       </c>
       <c r="G24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="H24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
         <v>69</v>
       </c>
       <c r="D25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" t="s">
         <v>98</v>
       </c>
-      <c r="E25" t="s">
-        <v>90</v>
-      </c>
       <c r="F25" t="s">
         <v>73</v>
       </c>
-      <c r="G25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
         <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="E26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C27" t="s">
         <v>69</v>
       </c>
       <c r="D27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
         <v>69</v>
       </c>
       <c r="D28" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="E28" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C29" t="s">
         <v>69</v>
       </c>
       <c r="D29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="E29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
         <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E30" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
         <v>69</v>
       </c>
       <c r="D31" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" t="s">
         <v>96</v>
       </c>
-      <c r="E31" t="s">
-        <v>80</v>
-      </c>
       <c r="F31" t="s">
         <v>73</v>
       </c>
       <c r="G31" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="H31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
         <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
         <v>69</v>
       </c>
       <c r="D33" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E33" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" t="s">
+        <v>73</v>
+      </c>
+      <c r="H33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
         <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E34" t="s">
         <v>73</v>
@@ -1418,35 +1542,38 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
         <v>70</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E35" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
         <v>70</v>
       </c>
       <c r="D36" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E36" t="s">
         <v>73</v>
@@ -1455,69 +1582,84 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
         <v>70</v>
       </c>
       <c r="D37" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E37" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
         <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E38" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C39" t="s">
         <v>69</v>
       </c>
       <c r="D39" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E39" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>73</v>
+      </c>
+      <c r="G39" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
         <v>70</v>
       </c>
       <c r="D40" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E40" t="s">
         <v>73</v>
@@ -1526,205 +1668,265 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C41" t="s">
         <v>70</v>
       </c>
       <c r="D41" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E41" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>73</v>
+      </c>
+      <c r="G41" t="s">
+        <v>73</v>
+      </c>
+      <c r="H41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C42" t="s">
         <v>70</v>
       </c>
       <c r="D42" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E42" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C43" t="s">
         <v>70</v>
       </c>
       <c r="D43" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E43" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
         <v>71</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E44" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="F44" t="s">
+        <v>73</v>
       </c>
       <c r="G44" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="H44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
         <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="E45" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" t="s">
+        <v>73</v>
+      </c>
+      <c r="G45" t="s">
+        <v>73</v>
+      </c>
+      <c r="H45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
         <v>72</v>
       </c>
       <c r="D46" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="E46" t="s">
+        <v>84</v>
+      </c>
+      <c r="F46" t="s">
+        <v>73</v>
+      </c>
+      <c r="G46" t="s">
+        <v>73</v>
+      </c>
+      <c r="H46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C47" t="s">
         <v>72</v>
       </c>
       <c r="D47" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E47" t="s">
-        <v>76</v>
-      </c>
-      <c r="G47" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="F47" t="s">
+        <v>73</v>
+      </c>
+      <c r="H47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s">
         <v>72</v>
       </c>
       <c r="D48" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E48" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="F48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
         <v>72</v>
       </c>
       <c r="D49" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E49" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="F49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C50" t="s">
         <v>72</v>
       </c>
       <c r="D50" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E50" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="F50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C51" t="s">
         <v>72</v>
       </c>
       <c r="D51" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E51" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="F51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C52" t="s">
         <v>71</v>
       </c>
       <c r="D52" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E52" t="s">
         <v>73</v>
@@ -1733,72 +1935,87 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C53" t="s">
         <v>71</v>
       </c>
       <c r="D53" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E53" t="s">
-        <v>89</v>
-      </c>
-      <c r="G53" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="F53" t="s">
+        <v>73</v>
+      </c>
+      <c r="H53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C54" t="s">
         <v>69</v>
       </c>
       <c r="D54" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E54" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>73</v>
+      </c>
+      <c r="G54" t="s">
+        <v>73</v>
+      </c>
+      <c r="H54" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C55" t="s">
         <v>71</v>
       </c>
       <c r="D55" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E55" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C56" t="s">
         <v>71</v>
       </c>
       <c r="D56" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E56" t="s">
         <v>73</v>
@@ -1807,203 +2024,242 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C57" t="s">
         <v>71</v>
       </c>
       <c r="D57" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E57" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F57" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C58" t="s">
         <v>71</v>
       </c>
       <c r="D58" t="s">
+        <v>89</v>
+      </c>
+      <c r="E58" t="s">
         <v>96</v>
       </c>
-      <c r="E58" t="s">
-        <v>80</v>
-      </c>
       <c r="F58" t="s">
         <v>73</v>
       </c>
       <c r="G58" t="s">
+        <v>73</v>
+      </c>
+      <c r="H58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>99</v>
-      </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C59" t="s">
         <v>71</v>
       </c>
       <c r="D59" t="s">
+        <v>89</v>
+      </c>
+      <c r="E59" t="s">
         <v>96</v>
       </c>
-      <c r="E59" t="s">
-        <v>80</v>
-      </c>
       <c r="F59" t="s">
         <v>73</v>
       </c>
       <c r="G59" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="H59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C60" t="s">
         <v>71</v>
       </c>
       <c r="D60" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E60" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F60" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C61" t="s">
         <v>71</v>
       </c>
       <c r="D61" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E61" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F61" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C62" t="s">
         <v>71</v>
       </c>
       <c r="D62" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E62" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F62" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>59</v>
       </c>
       <c r="B63" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
         <v>71</v>
       </c>
       <c r="D63" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E63" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F63" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C64" t="s">
         <v>71</v>
       </c>
       <c r="D64" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E64" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F64" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C65" t="s">
         <v>71</v>
       </c>
       <c r="D65" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E65" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F65" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C66" t="s">
         <v>71</v>
       </c>
       <c r="D66" t="s">
-        <v>98</v>
+        <v>91</v>
+      </c>
+      <c r="E66" t="s">
+        <v>97</v>
       </c>
       <c r="G66" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="H66" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>63</v>
       </c>
       <c r="B67" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C67" t="s">
         <v>71</v>
       </c>
       <c r="D67" t="s">
-        <v>98</v>
+        <v>91</v>
+      </c>
+      <c r="E67" t="s">
+        <v>97</v>
       </c>
       <c r="G67" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="H67" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up pairplot and heatmap, added use_this_function parameter
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19626651-D2EE-42F8-9A67-2D2056A934D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A422A84-2A26-42A7-9D18-C26C94B09D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$67</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -95,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="106">
   <si>
     <t>row_id</t>
   </si>
@@ -789,8 +792,8 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,7 +802,7 @@
     <col min="2" max="2" width="23.88671875" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="27.5546875" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" customWidth="1"/>
     <col min="7" max="7" width="18.88671875" customWidth="1"/>
     <col min="8" max="8" width="39.77734375" customWidth="1"/>
@@ -833,36 +836,30 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
         <v>88</v>
@@ -876,27 +873,30 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" t="s">
-        <v>73</v>
+        <v>97</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>79</v>
@@ -916,7 +916,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>79</v>
@@ -930,13 +930,10 @@
       <c r="E6" t="s">
         <v>73</v>
       </c>
-      <c r="F6" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>79</v>
@@ -956,7 +953,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>79</v>
@@ -976,7 +973,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>79</v>
@@ -996,7 +993,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>79</v>
@@ -1016,47 +1013,50 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="F12" t="s">
         <v>73</v>
+      </c>
+      <c r="G12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>79</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
         <v>79</v>
@@ -1096,13 +1096,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
         <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
         <v>88</v>
@@ -1113,45 +1113,54 @@
       <c r="F15" t="s">
         <v>73</v>
       </c>
+      <c r="G15" t="s">
+        <v>73</v>
+      </c>
       <c r="H15" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="F16" t="s">
         <v>73</v>
+      </c>
+      <c r="G16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
         <v>73</v>
@@ -1159,19 +1168,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
         <v>73</v>
@@ -1179,19 +1188,19 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
         <v>73</v>
@@ -1199,19 +1208,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F20" t="s">
         <v>73</v>
@@ -1219,220 +1228,208 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F21" t="s">
         <v>73</v>
+      </c>
+      <c r="H21" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="F23" t="s">
         <v>73</v>
+      </c>
+      <c r="G23" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
         <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s">
-        <v>97</v>
-      </c>
-      <c r="F24" t="s">
         <v>73</v>
       </c>
       <c r="G24" t="s">
         <v>73</v>
       </c>
       <c r="H24" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
         <v>81</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
         <v>91</v>
       </c>
       <c r="E25" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F25" t="s">
         <v>73</v>
       </c>
+      <c r="G25" t="s">
+        <v>73</v>
+      </c>
       <c r="H25" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
         <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
         <v>91</v>
       </c>
       <c r="E26" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="F26" t="s">
         <v>73</v>
       </c>
       <c r="G26" t="s">
         <v>73</v>
+      </c>
+      <c r="H26" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E27" t="s">
-        <v>97</v>
-      </c>
-      <c r="F27" t="s">
-        <v>73</v>
-      </c>
-      <c r="G27" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="F28" t="s">
         <v>73</v>
-      </c>
-      <c r="G28" t="s">
-        <v>73</v>
-      </c>
-      <c r="H28" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E29" t="s">
-        <v>97</v>
-      </c>
-      <c r="F29" t="s">
-        <v>73</v>
-      </c>
-      <c r="G29" t="s">
-        <v>73</v>
-      </c>
-      <c r="H29" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30" t="s">
         <v>88</v>
@@ -1446,111 +1443,93 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E31" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="F31" t="s">
         <v>73</v>
-      </c>
-      <c r="G31" t="s">
-        <v>73</v>
-      </c>
-      <c r="H31" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D32" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E32" t="s">
         <v>73</v>
-      </c>
-      <c r="F32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H32" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E33" t="s">
         <v>73</v>
       </c>
       <c r="F33" t="s">
         <v>73</v>
-      </c>
-      <c r="G33" t="s">
-        <v>73</v>
-      </c>
-      <c r="H33" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
         <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E34" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="F34" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D35" t="s">
         <v>88</v>
@@ -1564,99 +1543,93 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D37" t="s">
         <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>73</v>
-      </c>
-      <c r="F37" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
         <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E38" t="s">
-        <v>73</v>
-      </c>
-      <c r="F38" t="s">
-        <v>73</v>
+        <v>97</v>
+      </c>
+      <c r="G38" t="s">
+        <v>73</v>
+      </c>
+      <c r="H38" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
         <v>69</v>
       </c>
       <c r="D39" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E39" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="F39" t="s">
         <v>73</v>
       </c>
-      <c r="G39" t="s">
-        <v>73</v>
-      </c>
       <c r="H39" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
         <v>89</v>
@@ -1666,23 +1639,29 @@
       </c>
       <c r="F40" t="s">
         <v>73</v>
+      </c>
+      <c r="G40" t="s">
+        <v>73</v>
+      </c>
+      <c r="H40" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
         <v>89</v>
       </c>
       <c r="E41" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="F41" t="s">
         <v>73</v>
@@ -1691,32 +1670,32 @@
         <v>73</v>
       </c>
       <c r="H41" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E42" t="s">
         <v>73</v>
       </c>
-      <c r="F42" t="s">
-        <v>73</v>
+      <c r="H42" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
         <v>100</v>
@@ -1730,25 +1709,22 @@
       <c r="E43" t="s">
         <v>73</v>
       </c>
-      <c r="F43" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D44" t="s">
         <v>91</v>
       </c>
       <c r="E44" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F44" t="s">
         <v>73</v>
@@ -1757,99 +1733,84 @@
         <v>73</v>
       </c>
       <c r="H44" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="C45" t="s">
         <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E45" t="s">
-        <v>84</v>
-      </c>
-      <c r="F45" t="s">
         <v>73</v>
       </c>
       <c r="G45" t="s">
         <v>73</v>
       </c>
       <c r="H45" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B46" t="s">
         <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D46" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E46" t="s">
-        <v>84</v>
-      </c>
-      <c r="F46" t="s">
-        <v>73</v>
-      </c>
-      <c r="G46" t="s">
-        <v>73</v>
-      </c>
-      <c r="H46" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
         <v>89</v>
       </c>
       <c r="E47" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="F47" t="s">
         <v>73</v>
-      </c>
-      <c r="H47" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D48" t="s">
         <v>89</v>
       </c>
       <c r="E48" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="F48" t="s">
         <v>73</v>
@@ -1857,19 +1818,19 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C49" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E49" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="F49" t="s">
         <v>73</v>
@@ -1877,188 +1838,167 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E50" t="s">
-        <v>103</v>
-      </c>
-      <c r="F50" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E51" t="s">
-        <v>103</v>
-      </c>
-      <c r="F51" t="s">
-        <v>73</v>
+        <v>73</v>
+      </c>
+      <c r="H51" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C52" t="s">
         <v>71</v>
       </c>
       <c r="D52" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E52" t="s">
-        <v>73</v>
-      </c>
-      <c r="F52" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C53" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D53" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E53" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="F53" t="s">
         <v>73</v>
       </c>
+      <c r="G53" t="s">
+        <v>73</v>
+      </c>
       <c r="H53" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D54" t="s">
         <v>88</v>
       </c>
       <c r="E54" t="s">
         <v>73</v>
-      </c>
-      <c r="F54" t="s">
-        <v>73</v>
-      </c>
-      <c r="G54" t="s">
-        <v>73</v>
-      </c>
-      <c r="H54" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D55" t="s">
         <v>88</v>
       </c>
       <c r="E55" t="s">
-        <v>73</v>
-      </c>
-      <c r="F55" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C56" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E56" t="s">
-        <v>73</v>
-      </c>
-      <c r="F56" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C57" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D57" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E57" t="s">
-        <v>73</v>
-      </c>
-      <c r="F57" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B58" t="s">
         <v>81</v>
       </c>
       <c r="C58" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E58" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="F58" t="s">
         <v>73</v>
@@ -2067,98 +2007,86 @@
         <v>73</v>
       </c>
       <c r="H58" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E59" t="s">
-        <v>96</v>
-      </c>
-      <c r="F59" t="s">
-        <v>73</v>
-      </c>
-      <c r="G59" t="s">
-        <v>73</v>
-      </c>
-      <c r="H59" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D60" t="s">
         <v>89</v>
       </c>
       <c r="E60" t="s">
-        <v>73</v>
-      </c>
-      <c r="F60" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C61" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E61" t="s">
-        <v>73</v>
-      </c>
-      <c r="F61" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="B62" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C62" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D62" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E62" t="s">
-        <v>73</v>
-      </c>
-      <c r="F62" t="s">
-        <v>73</v>
+        <v>97</v>
+      </c>
+      <c r="G62" t="s">
+        <v>73</v>
+      </c>
+      <c r="H62" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
         <v>82</v>
@@ -2172,22 +2100,19 @@
       <c r="E63" t="s">
         <v>73</v>
       </c>
-      <c r="F63" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B64" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C64" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E64" t="s">
         <v>73</v>
@@ -2198,10 +2123,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C65" t="s">
         <v>71</v>
@@ -2210,21 +2135,27 @@
         <v>89</v>
       </c>
       <c r="E65" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="F65" t="s">
         <v>73</v>
+      </c>
+      <c r="G65" t="s">
+        <v>73</v>
+      </c>
+      <c r="H65" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="B66" t="s">
         <v>81</v>
       </c>
       <c r="C66" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D66" t="s">
         <v>91</v>
@@ -2232,37 +2163,39 @@
       <c r="E66" t="s">
         <v>97</v>
       </c>
+      <c r="F66" t="s">
+        <v>73</v>
+      </c>
       <c r="G66" t="s">
         <v>73</v>
-      </c>
-      <c r="H66" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="B67" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C67" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D67" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E67" t="s">
-        <v>97</v>
-      </c>
-      <c r="G67" t="s">
-        <v>73</v>
-      </c>
-      <c r="H67" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="F67" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H67" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H67">
+      <sortCondition ref="A1:A67"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
added DBSCAN to clustering
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A422A84-2A26-42A7-9D18-C26C94B09D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D8FCEA-31EB-4D77-8158-DF84B085CCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -792,8 +792,8 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added create_classification_models_overview() to compare models settings
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D8FCEA-31EB-4D77-8158-DF84B085CCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0099667-F319-4F89-8212-B449E15B7FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -792,8 +792,8 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added accuracy, recall, precision to compare_classification_models_on_cohort(), also reworked confusion matrix plot
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0099667-F319-4F89-8212-B449E15B7FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7467909-7AC9-4A41-83B0-359F5E4E3704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -792,8 +792,8 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
started with categorical correlation, still not working
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7467909-7AC9-4A41-83B0-359F5E4E3704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BDEBF3-28D9-4C7C-879E-5FFE6D3A1C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="108">
   <si>
     <t>row_id</t>
   </si>
@@ -416,6 +416,12 @@
   </si>
   <si>
     <t>not remove because needed in clustering, but remove in python for correlation &amp; classification</t>
+  </si>
+  <si>
+    <t>old_selection</t>
+  </si>
+  <si>
+    <t>USEFUL? OR NOT CORRECT?</t>
   </si>
 </sst>
 </file>
@@ -789,11 +795,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -808,7 +814,7 @@
     <col min="8" max="8" width="39.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
@@ -833,8 +839,11 @@
       <c r="H1" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -851,129 +860,129 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
         <v>70</v>
       </c>
-      <c r="D3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" t="s">
-        <v>71</v>
-      </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>79</v>
@@ -990,10 +999,13 @@
       <c r="F9" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>79</v>
@@ -1007,56 +1019,56 @@
       <c r="E10" t="s">
         <v>73</v>
       </c>
-      <c r="F10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="F12" t="s">
         <v>73</v>
       </c>
-      <c r="G12" t="s">
-        <v>73</v>
-      </c>
-      <c r="H12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>79</v>
@@ -1073,10 +1085,13 @@
       <c r="F13" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>79</v>
@@ -1093,337 +1108,337 @@
       <c r="F14" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" t="s">
         <v>69</v>
       </c>
-      <c r="D15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="D17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" t="s">
-        <v>96</v>
-      </c>
-      <c r="F16" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" t="s">
-        <v>103</v>
-      </c>
-      <c r="F17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="F18" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="F19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="F20" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="F21" t="s">
         <v>73</v>
       </c>
-      <c r="H21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
         <v>71</v>
       </c>
-      <c r="D22" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" t="s">
+        <v>107</v>
+      </c>
+      <c r="I25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
         <v>71</v>
       </c>
-      <c r="D23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" t="s">
-        <v>84</v>
-      </c>
-      <c r="F23" t="s">
-        <v>73</v>
-      </c>
-      <c r="G23" t="s">
-        <v>73</v>
-      </c>
-      <c r="H23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" t="s">
-        <v>84</v>
-      </c>
-      <c r="F25" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" t="s">
-        <v>73</v>
-      </c>
-      <c r="H25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" t="s">
-        <v>72</v>
-      </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26" t="s">
-        <v>73</v>
-      </c>
-      <c r="G26" t="s">
         <v>73</v>
       </c>
       <c r="H26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E27" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E28" t="s">
         <v>73</v>
       </c>
-      <c r="F28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
         <v>79</v>
@@ -1437,19 +1452,16 @@
       <c r="E30" t="s">
         <v>73</v>
       </c>
-      <c r="F30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
         <v>88</v>
@@ -1457,30 +1469,33 @@
       <c r="E31" t="s">
         <v>73</v>
       </c>
-      <c r="F31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E32" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
+      <c r="I32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
         <v>79</v>
@@ -1497,42 +1512,42 @@
       <c r="F33" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E34" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="F34" t="s">
         <v>73</v>
       </c>
-      <c r="G34" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E35" t="s">
         <v>73</v>
@@ -1541,26 +1556,29 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D36" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E36" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
         <v>82</v>
@@ -1574,62 +1592,65 @@
       <c r="E37" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>73</v>
+      </c>
+      <c r="I37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
         <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E38" t="s">
-        <v>97</v>
-      </c>
-      <c r="G38" t="s">
-        <v>73</v>
-      </c>
-      <c r="H38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="F38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D39" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E39" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="F39" t="s">
         <v>73</v>
       </c>
-      <c r="H39" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D40" t="s">
         <v>89</v>
@@ -1640,19 +1661,13 @@
       <c r="F40" t="s">
         <v>73</v>
       </c>
-      <c r="G40" t="s">
-        <v>73</v>
-      </c>
-      <c r="H40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C41" t="s">
         <v>71</v>
@@ -1661,61 +1676,76 @@
         <v>89</v>
       </c>
       <c r="E41" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="F41" t="s">
         <v>73</v>
       </c>
-      <c r="G41" t="s">
-        <v>73</v>
-      </c>
-      <c r="H41" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D42" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E42" t="s">
+        <v>97</v>
+      </c>
+      <c r="F42" t="s">
+        <v>73</v>
+      </c>
+      <c r="G42" t="s">
         <v>73</v>
       </c>
       <c r="H42" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="I42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E43" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="F43" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" t="s">
+        <v>73</v>
+      </c>
+      <c r="H43" t="s">
+        <v>74</v>
+      </c>
+      <c r="I43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
         <v>69</v>
@@ -1726,185 +1756,218 @@
       <c r="E44" t="s">
         <v>97</v>
       </c>
-      <c r="F44" t="s">
-        <v>73</v>
-      </c>
       <c r="G44" t="s">
         <v>73</v>
       </c>
       <c r="H44" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
         <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E45" t="s">
         <v>73</v>
       </c>
-      <c r="G45" t="s">
-        <v>73</v>
-      </c>
-      <c r="H45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F45" t="s">
+        <v>73</v>
+      </c>
+      <c r="I45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
         <v>81</v>
       </c>
       <c r="C46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" t="s">
+        <v>97</v>
+      </c>
+      <c r="G46" t="s">
+        <v>73</v>
+      </c>
+      <c r="H46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" t="s">
         <v>69</v>
       </c>
-      <c r="D46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E46" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" t="s">
-        <v>70</v>
-      </c>
       <c r="D47" t="s">
         <v>89</v>
       </c>
       <c r="E47" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="F47" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H47" t="s">
+        <v>99</v>
+      </c>
+      <c r="I47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D48" t="s">
         <v>89</v>
       </c>
       <c r="E48" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F48" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D49" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E49" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F49" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D50" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E50" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="F50" t="s">
+        <v>73</v>
+      </c>
+      <c r="I50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C51" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D51" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E51" t="s">
-        <v>73</v>
-      </c>
-      <c r="H51" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="F51" t="s">
+        <v>73</v>
+      </c>
+      <c r="I51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D52" t="s">
         <v>89</v>
       </c>
       <c r="E52" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="F52" t="s">
+        <v>73</v>
+      </c>
+      <c r="H52" t="s">
+        <v>86</v>
+      </c>
+      <c r="I52" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B53" t="s">
         <v>81</v>
       </c>
       <c r="C53" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D53" t="s">
         <v>91</v>
       </c>
       <c r="E53" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="F53" t="s">
         <v>73</v>
@@ -1915,27 +1978,42 @@
       <c r="H53" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C54" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D54" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E54" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="F54" t="s">
+        <v>73</v>
+      </c>
+      <c r="G54" t="s">
+        <v>73</v>
+      </c>
+      <c r="H54" t="s">
+        <v>101</v>
+      </c>
+      <c r="I54" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B55" t="s">
         <v>81</v>
@@ -1944,49 +2022,64 @@
         <v>70</v>
       </c>
       <c r="D55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E55" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B56" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C56" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D56" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E56" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="F56" t="s">
+        <v>73</v>
+      </c>
+      <c r="G56" t="s">
+        <v>73</v>
+      </c>
+      <c r="I56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="B57" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C57" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D57" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E57" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="G57" t="s">
+        <v>73</v>
+      </c>
+      <c r="H57" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="B58" t="s">
         <v>81</v>
@@ -1995,121 +2088,163 @@
         <v>69</v>
       </c>
       <c r="D58" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E58" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="F58" t="s">
         <v>73</v>
       </c>
-      <c r="G58" t="s">
-        <v>73</v>
-      </c>
       <c r="H58" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="I58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B59" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C59" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D59" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E59" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F59" t="s">
+        <v>73</v>
+      </c>
+      <c r="G59" t="s">
+        <v>73</v>
+      </c>
+      <c r="H59" t="s">
+        <v>104</v>
+      </c>
+      <c r="I59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="B60" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C60" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D60" t="s">
         <v>89</v>
       </c>
       <c r="E60" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="F60" t="s">
+        <v>73</v>
+      </c>
+      <c r="G60" t="s">
+        <v>73</v>
+      </c>
+      <c r="H60" t="s">
+        <v>93</v>
+      </c>
+      <c r="I60" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B61" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C61" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D61" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E61" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="F61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G61" t="s">
+        <v>73</v>
+      </c>
+      <c r="H61" t="s">
+        <v>101</v>
+      </c>
+      <c r="I61" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C62" t="s">
         <v>69</v>
       </c>
       <c r="D62" t="s">
+        <v>88</v>
+      </c>
+      <c r="E62" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" t="s">
+        <v>69</v>
+      </c>
+      <c r="D63" t="s">
         <v>91</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E63" t="s">
         <v>97</v>
       </c>
-      <c r="G62" t="s">
-        <v>73</v>
-      </c>
-      <c r="H62" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>61</v>
-      </c>
-      <c r="B63" t="s">
-        <v>82</v>
-      </c>
-      <c r="C63" t="s">
-        <v>71</v>
-      </c>
-      <c r="D63" t="s">
-        <v>89</v>
-      </c>
-      <c r="E63" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F63" t="s">
+        <v>73</v>
+      </c>
+      <c r="G63" t="s">
+        <v>73</v>
+      </c>
+      <c r="H63" t="s">
+        <v>101</v>
+      </c>
+      <c r="I63" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C64" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D64" t="s">
         <v>88</v>
@@ -2117,25 +2252,22 @@
       <c r="E64" t="s">
         <v>73</v>
       </c>
-      <c r="F64" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B65" t="s">
         <v>81</v>
       </c>
       <c r="C65" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E65" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="F65" t="s">
         <v>73</v>
@@ -2144,56 +2276,68 @@
         <v>73</v>
       </c>
       <c r="H65" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="I65" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B66" t="s">
         <v>81</v>
       </c>
       <c r="C66" t="s">
+        <v>71</v>
+      </c>
+      <c r="D66" t="s">
+        <v>89</v>
+      </c>
+      <c r="E66" t="s">
+        <v>96</v>
+      </c>
+      <c r="F66" t="s">
+        <v>73</v>
+      </c>
+      <c r="H66" t="s">
+        <v>85</v>
+      </c>
+      <c r="I66" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" t="s">
         <v>69</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>91</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E67" t="s">
         <v>97</v>
       </c>
-      <c r="F66" t="s">
-        <v>73</v>
-      </c>
-      <c r="G66" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>21</v>
-      </c>
-      <c r="B67" t="s">
-        <v>79</v>
-      </c>
-      <c r="C67" t="s">
-        <v>68</v>
-      </c>
-      <c r="D67" t="s">
-        <v>88</v>
-      </c>
-      <c r="E67" t="s">
-        <v>73</v>
-      </c>
       <c r="F67" t="s">
         <v>73</v>
       </c>
+      <c r="G67" t="s">
+        <v>73</v>
+      </c>
+      <c r="I67" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H67" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H67">
-      <sortCondition ref="A1:A67"/>
+  <autoFilter ref="A1:I1" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I67">
+      <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added outliers removal for avg_cohort, bit less data but better data
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BDEBF3-28D9-4C7C-879E-5FFE6D3A1C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED1843F-5DFE-49F4-9B4B-E17590B9EDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="108">
   <si>
     <t>row_id</t>
   </si>
@@ -798,8 +798,8 @@
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -862,96 +862,102 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
         <v>73</v>
       </c>
-      <c r="G3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" t="s">
-        <v>104</v>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>97</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E6" t="s">
         <v>73</v>
-      </c>
-      <c r="G6" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" t="s">
         <v>73</v>
@@ -965,24 +971,30 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>79</v>
@@ -1005,7 +1017,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>79</v>
@@ -1019,48 +1031,57 @@
       <c r="E10" t="s">
         <v>73</v>
       </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E11" t="s">
         <v>73</v>
       </c>
       <c r="F11" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="F12" t="s">
         <v>73</v>
+      </c>
+      <c r="G12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" t="s">
+        <v>101</v>
       </c>
       <c r="I12" t="s">
         <v>73</v>
@@ -1068,7 +1089,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>79</v>
@@ -1091,7 +1112,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
         <v>79</v>
@@ -1114,13 +1135,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
         <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
         <v>88</v>
@@ -1130,6 +1151,12 @@
       </c>
       <c r="F15" t="s">
         <v>73</v>
+      </c>
+      <c r="G15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" t="s">
+        <v>104</v>
       </c>
       <c r="I15" t="s">
         <v>73</v>
@@ -1137,22 +1164,25 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="F16" t="s">
         <v>73</v>
+      </c>
+      <c r="H16" t="s">
+        <v>99</v>
       </c>
       <c r="I16" t="s">
         <v>73</v>
@@ -1160,28 +1190,22 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
         <v>73</v>
-      </c>
-      <c r="G17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" t="s">
-        <v>104</v>
       </c>
       <c r="I17" t="s">
         <v>73</v>
@@ -1189,19 +1213,19 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
         <v>73</v>
@@ -1212,19 +1236,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
         <v>73</v>
@@ -1235,19 +1259,19 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F20" t="s">
         <v>73</v>
@@ -1258,22 +1282,25 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F21" t="s">
         <v>73</v>
+      </c>
+      <c r="H21" t="s">
+        <v>86</v>
       </c>
       <c r="I21" t="s">
         <v>73</v>
@@ -1281,85 +1308,100 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E23" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" t="s">
         <v>73</v>
       </c>
       <c r="H23" t="s">
-        <v>90</v>
+        <v>74</v>
+      </c>
+      <c r="I23" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s">
         <v>73</v>
       </c>
-      <c r="F24" t="s">
-        <v>73</v>
-      </c>
-      <c r="I24" t="s">
-        <v>73</v>
+      <c r="G24" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="F25" t="s">
         <v>73</v>
       </c>
+      <c r="G25" t="s">
+        <v>73</v>
+      </c>
       <c r="H25" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="I25" t="s">
         <v>73</v>
@@ -1367,70 +1409,88 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" t="s">
         <v>73</v>
       </c>
       <c r="H26" t="s">
-        <v>75</v>
+        <v>101</v>
+      </c>
+      <c r="I26" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E29" t="s">
         <v>73</v>
@@ -1438,7 +1498,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
         <v>79</v>
@@ -1452,36 +1512,48 @@
       <c r="E30" t="s">
         <v>73</v>
       </c>
+      <c r="F30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D31" t="s">
         <v>88</v>
       </c>
       <c r="E31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D32" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E32" t="s">
         <v>73</v>
@@ -1495,7 +1567,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B33" t="s">
         <v>79</v>
@@ -1518,67 +1590,73 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E34" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="F34" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E35" t="s">
         <v>73</v>
       </c>
       <c r="F35" t="s">
+        <v>73</v>
+      </c>
+      <c r="I35" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
         <v>82</v>
@@ -1595,48 +1673,51 @@
       <c r="F37" t="s">
         <v>73</v>
       </c>
-      <c r="I37" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
         <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E38" t="s">
-        <v>73</v>
-      </c>
-      <c r="F38" t="s">
-        <v>73</v>
+        <v>97</v>
+      </c>
+      <c r="G38" t="s">
+        <v>73</v>
+      </c>
+      <c r="H38" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D39" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E39" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="F39" t="s">
         <v>73</v>
+      </c>
+      <c r="H39" t="s">
+        <v>105</v>
       </c>
       <c r="I39" t="s">
         <v>73</v>
@@ -1644,13 +1725,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
         <v>89</v>
@@ -1659,15 +1740,24 @@
         <v>73</v>
       </c>
       <c r="F40" t="s">
+        <v>73</v>
+      </c>
+      <c r="G40" t="s">
+        <v>73</v>
+      </c>
+      <c r="H40" t="s">
+        <v>104</v>
+      </c>
+      <c r="I40" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
         <v>71</v>
@@ -1676,76 +1766,64 @@
         <v>89</v>
       </c>
       <c r="E41" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="F41" t="s">
+        <v>73</v>
+      </c>
+      <c r="G41" t="s">
+        <v>73</v>
+      </c>
+      <c r="H41" t="s">
+        <v>93</v>
+      </c>
+      <c r="I41" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D42" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E42" t="s">
-        <v>97</v>
-      </c>
-      <c r="F42" t="s">
-        <v>73</v>
-      </c>
-      <c r="G42" t="s">
         <v>73</v>
       </c>
       <c r="H42" t="s">
-        <v>101</v>
-      </c>
-      <c r="I42" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E43" t="s">
-        <v>84</v>
-      </c>
-      <c r="F43" t="s">
-        <v>73</v>
-      </c>
-      <c r="G43" t="s">
-        <v>73</v>
-      </c>
-      <c r="H43" t="s">
-        <v>74</v>
-      </c>
-      <c r="I43" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
         <v>69</v>
@@ -1756,80 +1834,77 @@
       <c r="E44" t="s">
         <v>97</v>
       </c>
+      <c r="F44" t="s">
+        <v>73</v>
+      </c>
       <c r="G44" t="s">
         <v>73</v>
       </c>
       <c r="H44" t="s">
-        <v>77</v>
+        <v>101</v>
+      </c>
+      <c r="I44" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="C45" t="s">
         <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E45" t="s">
         <v>73</v>
       </c>
-      <c r="F45" t="s">
-        <v>73</v>
-      </c>
-      <c r="I45" t="s">
-        <v>73</v>
+      <c r="G45" t="s">
+        <v>73</v>
+      </c>
+      <c r="H45" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B46" t="s">
         <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D46" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E46" t="s">
-        <v>97</v>
-      </c>
-      <c r="G46" t="s">
-        <v>73</v>
-      </c>
-      <c r="H46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
         <v>89</v>
       </c>
       <c r="E47" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="F47" t="s">
         <v>73</v>
-      </c>
-      <c r="H47" t="s">
-        <v>99</v>
       </c>
       <c r="I47" t="s">
         <v>73</v>
@@ -1837,19 +1912,19 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D48" t="s">
         <v>89</v>
       </c>
       <c r="E48" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="F48" t="s">
         <v>73</v>
@@ -1860,19 +1935,19 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C49" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E49" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="F49" t="s">
         <v>73</v>
@@ -1883,22 +1958,25 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E50" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="F50" t="s">
         <v>73</v>
+      </c>
+      <c r="H50" t="s">
+        <v>107</v>
       </c>
       <c r="I50" t="s">
         <v>73</v>
@@ -1906,68 +1984,59 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E51" t="s">
-        <v>103</v>
-      </c>
-      <c r="F51" t="s">
-        <v>73</v>
-      </c>
-      <c r="I51" t="s">
-        <v>73</v>
+        <v>73</v>
+      </c>
+      <c r="H51" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D52" t="s">
         <v>89</v>
       </c>
       <c r="E52" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="F52" t="s">
-        <v>73</v>
-      </c>
-      <c r="H52" t="s">
-        <v>86</v>
-      </c>
-      <c r="I52" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s">
         <v>81</v>
       </c>
       <c r="C53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D53" t="s">
         <v>91</v>
       </c>
       <c r="E53" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F53" t="s">
         <v>73</v>
@@ -1984,36 +2053,27 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C54" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D54" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E54" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F54" t="s">
-        <v>73</v>
-      </c>
-      <c r="G54" t="s">
-        <v>73</v>
-      </c>
-      <c r="H54" t="s">
-        <v>101</v>
-      </c>
-      <c r="I54" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B55" t="s">
         <v>81</v>
@@ -2022,64 +2082,52 @@
         <v>70</v>
       </c>
       <c r="D55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E55" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D56" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E56" t="s">
-        <v>97</v>
-      </c>
-      <c r="F56" t="s">
-        <v>73</v>
-      </c>
-      <c r="G56" t="s">
-        <v>73</v>
-      </c>
-      <c r="I56" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C57" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D57" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E57" t="s">
-        <v>97</v>
-      </c>
-      <c r="G57" t="s">
-        <v>73</v>
-      </c>
-      <c r="H57" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B58" t="s">
         <v>81</v>
@@ -2088,16 +2136,19 @@
         <v>69</v>
       </c>
       <c r="D58" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E58" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="F58" t="s">
         <v>73</v>
       </c>
+      <c r="G58" t="s">
+        <v>73</v>
+      </c>
       <c r="H58" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I58" t="s">
         <v>73</v>
@@ -2105,178 +2156,142 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E59" t="s">
-        <v>73</v>
-      </c>
-      <c r="F59" t="s">
-        <v>73</v>
-      </c>
-      <c r="G59" t="s">
-        <v>73</v>
-      </c>
-      <c r="H59" t="s">
-        <v>104</v>
-      </c>
-      <c r="I59" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="B60" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="C60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D60" t="s">
         <v>89</v>
       </c>
       <c r="E60" t="s">
-        <v>96</v>
-      </c>
-      <c r="F60" t="s">
-        <v>73</v>
-      </c>
-      <c r="G60" t="s">
-        <v>73</v>
-      </c>
-      <c r="H60" t="s">
-        <v>93</v>
-      </c>
-      <c r="I60" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D61" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E61" t="s">
-        <v>97</v>
-      </c>
-      <c r="F61" t="s">
-        <v>73</v>
-      </c>
-      <c r="G61" t="s">
-        <v>73</v>
-      </c>
-      <c r="H61" t="s">
-        <v>101</v>
-      </c>
-      <c r="I61" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="B62" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C62" t="s">
         <v>69</v>
       </c>
       <c r="D62" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E62" t="s">
-        <v>73</v>
+        <v>97</v>
+      </c>
+      <c r="G62" t="s">
+        <v>73</v>
+      </c>
+      <c r="H62" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D63" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E63" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="F63" t="s">
-        <v>73</v>
-      </c>
-      <c r="G63" t="s">
-        <v>73</v>
-      </c>
-      <c r="H63" t="s">
-        <v>101</v>
-      </c>
-      <c r="I63" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B64" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C64" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D64" t="s">
         <v>88</v>
       </c>
       <c r="E64" t="s">
+        <v>73</v>
+      </c>
+      <c r="F64" t="s">
+        <v>73</v>
+      </c>
+      <c r="I64" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
         <v>81</v>
       </c>
       <c r="C65" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D65" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E65" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="F65" t="s">
         <v>73</v>
       </c>
-      <c r="G65" t="s">
-        <v>73</v>
-      </c>
       <c r="H65" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="I65" t="s">
         <v>73</v>
@@ -2284,25 +2299,25 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="B66" t="s">
         <v>81</v>
       </c>
       <c r="C66" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D66" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E66" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F66" t="s">
         <v>73</v>
       </c>
-      <c r="H66" t="s">
-        <v>85</v>
+      <c r="G66" t="s">
+        <v>73</v>
       </c>
       <c r="I66" t="s">
         <v>73</v>
@@ -2310,24 +2325,21 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B67" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D67" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E67" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="F67" t="s">
-        <v>73</v>
-      </c>
-      <c r="G67" t="s">
         <v>73</v>
       </c>
       <c r="I67" t="s">
@@ -2337,7 +2349,7 @@
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I67">
-      <sortCondition ref="B1"/>
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added binary correlation, added FACTORIZATION_TABLE.xlsx instead of automatic factorization, plotted correlations for text, added function plot_random_forest with GridSearch for RF
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED1843F-5DFE-49F4-9B4B-E17590B9EDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC847A30-43E6-4318-9403-32E6CD836BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$J$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,6 +65,7 @@
           </rPr>
           <t xml:space="preserve">
 get item_id or unit-of-measurement from events_dictionary.xlsx
+important: when adding new features to the analysis make certain to also adjust the factorization table in supplements if the feature is categorical
 </t>
         </r>
       </text>
@@ -98,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="111">
   <si>
     <t>row_id</t>
   </si>
@@ -418,10 +419,19 @@
     <t>not remove because needed in clustering, but remove in python for correlation &amp; classification</t>
   </si>
   <si>
-    <t>old_selection</t>
-  </si>
-  <si>
     <t>USEFUL? OR NOT CORRECT?</t>
+  </si>
+  <si>
+    <t>only available in metavision</t>
+  </si>
+  <si>
+    <t>potentials_selection</t>
+  </si>
+  <si>
+    <t>strangely had no stat significance</t>
+  </si>
+  <si>
+    <t>final_selection_correlation</t>
   </si>
 </sst>
 </file>
@@ -458,12 +468,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -478,9 +494,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -795,26 +812,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="1" max="1" width="27.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" customWidth="1"/>
     <col min="7" max="7" width="18.88671875" customWidth="1"/>
     <col min="8" max="8" width="39.77734375" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
@@ -840,10 +859,13 @@
         <v>67</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -859,8 +881,14 @@
       <c r="E2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -876,14 +904,14 @@
       <c r="E3" t="s">
         <v>73</v>
       </c>
-      <c r="F3" t="s">
-        <v>73</v>
-      </c>
       <c r="I3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -899,6 +927,7 @@
       <c r="E4" t="s">
         <v>97</v>
       </c>
+      <c r="F4" s="2"/>
       <c r="G4" t="s">
         <v>73</v>
       </c>
@@ -906,7 +935,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -922,14 +951,14 @@
       <c r="E5" t="s">
         <v>73</v>
       </c>
-      <c r="F5" t="s">
-        <v>73</v>
-      </c>
       <c r="I5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -946,7 +975,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -962,14 +991,11 @@
       <c r="E7" t="s">
         <v>73</v>
       </c>
-      <c r="F7" t="s">
-        <v>73</v>
-      </c>
       <c r="I7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -985,14 +1011,8 @@
       <c r="E8" t="s">
         <v>73</v>
       </c>
-      <c r="F8" t="s">
-        <v>73</v>
-      </c>
-      <c r="I8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1014,8 +1034,11 @@
       <c r="I9" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1031,14 +1054,8 @@
       <c r="E10" t="s">
         <v>73</v>
       </c>
-      <c r="F10" t="s">
-        <v>73</v>
-      </c>
-      <c r="I10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1054,11 +1071,11 @@
       <c r="E11" t="s">
         <v>73</v>
       </c>
-      <c r="F11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1074,7 +1091,7 @@
       <c r="E12" t="s">
         <v>97</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G12" t="s">
@@ -1086,8 +1103,11 @@
       <c r="I12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1109,8 +1129,11 @@
       <c r="I13" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1126,14 +1149,14 @@
       <c r="E14" t="s">
         <v>73</v>
       </c>
-      <c r="F14" t="s">
-        <v>73</v>
-      </c>
       <c r="I14" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1149,7 +1172,7 @@
       <c r="E15" t="s">
         <v>73</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G15" t="s">
@@ -1161,8 +1184,11 @@
       <c r="I15" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -1178,7 +1204,7 @@
       <c r="E16" t="s">
         <v>96</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>73</v>
       </c>
       <c r="H16" t="s">
@@ -1187,8 +1213,11 @@
       <c r="I16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1204,14 +1233,17 @@
       <c r="E17" t="s">
         <v>103</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I17" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1227,14 +1259,17 @@
       <c r="E18" t="s">
         <v>103</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I18" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1250,14 +1285,17 @@
       <c r="E19" t="s">
         <v>103</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1273,14 +1311,17 @@
       <c r="E20" t="s">
         <v>103</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I20" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1296,7 +1337,7 @@
       <c r="E21" t="s">
         <v>103</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2" t="s">
         <v>73</v>
       </c>
       <c r="H21" t="s">
@@ -1305,8 +1346,11 @@
       <c r="I21" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1322,11 +1366,11 @@
       <c r="E22" t="s">
         <v>73</v>
       </c>
-      <c r="F22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1342,7 +1386,7 @@
       <c r="E23" t="s">
         <v>84</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G23" t="s">
@@ -1354,8 +1398,11 @@
       <c r="I23" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1371,6 +1418,7 @@
       <c r="E24" t="s">
         <v>73</v>
       </c>
+      <c r="F24" s="2"/>
       <c r="G24" t="s">
         <v>73</v>
       </c>
@@ -1378,7 +1426,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1394,7 +1442,7 @@
       <c r="E25" t="s">
         <v>84</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G25" t="s">
@@ -1406,8 +1454,11 @@
       <c r="I25" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1423,7 +1474,7 @@
       <c r="E26" t="s">
         <v>84</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G26" t="s">
@@ -1435,8 +1486,11 @@
       <c r="I26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1452,11 +1506,14 @@
       <c r="E27" t="s">
         <v>73</v>
       </c>
-      <c r="F27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I27" t="s">
+        <v>73</v>
+      </c>
+      <c r="J27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1472,14 +1529,14 @@
       <c r="E28" t="s">
         <v>73</v>
       </c>
-      <c r="F28" t="s">
-        <v>73</v>
-      </c>
       <c r="I28" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1496,7 +1553,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1512,14 +1569,11 @@
       <c r="E30" t="s">
         <v>73</v>
       </c>
-      <c r="F30" t="s">
-        <v>73</v>
-      </c>
       <c r="I30" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1541,8 +1595,11 @@
       <c r="I31" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1558,14 +1615,14 @@
       <c r="E32" t="s">
         <v>73</v>
       </c>
-      <c r="F32" t="s">
-        <v>73</v>
-      </c>
       <c r="I32" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1587,8 +1644,11 @@
       <c r="I33" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -1604,7 +1664,7 @@
       <c r="E34" t="s">
         <v>97</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G34" t="s">
@@ -1613,8 +1673,11 @@
       <c r="I34" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -1636,8 +1699,11 @@
       <c r="I35" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -1654,7 +1720,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -1670,11 +1736,11 @@
       <c r="E37" t="s">
         <v>73</v>
       </c>
-      <c r="F37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -1690,6 +1756,7 @@
       <c r="E38" t="s">
         <v>97</v>
       </c>
+      <c r="F38" s="2"/>
       <c r="G38" t="s">
         <v>73</v>
       </c>
@@ -1697,7 +1764,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -1713,7 +1780,7 @@
       <c r="E39" t="s">
         <v>98</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2" t="s">
         <v>73</v>
       </c>
       <c r="H39" t="s">
@@ -1722,8 +1789,11 @@
       <c r="I39" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -1739,7 +1809,7 @@
       <c r="E40" t="s">
         <v>73</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G40" t="s">
@@ -1751,8 +1821,11 @@
       <c r="I40" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -1768,7 +1841,7 @@
       <c r="E41" t="s">
         <v>96</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G41" t="s">
@@ -1780,8 +1853,11 @@
       <c r="I41" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -1797,11 +1873,14 @@
       <c r="E42" t="s">
         <v>73</v>
       </c>
+      <c r="F42" t="s">
+        <v>73</v>
+      </c>
       <c r="H42" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -1818,7 +1897,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -1834,7 +1913,7 @@
       <c r="E44" t="s">
         <v>97</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G44" t="s">
@@ -1846,8 +1925,11 @@
       <c r="I44" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -1863,6 +1945,7 @@
       <c r="E45" t="s">
         <v>73</v>
       </c>
+      <c r="F45" s="2"/>
       <c r="G45" t="s">
         <v>73</v>
       </c>
@@ -1870,7 +1953,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -1886,8 +1969,11 @@
       <c r="E46" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H46" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -1903,14 +1989,14 @@
       <c r="E47" t="s">
         <v>73</v>
       </c>
-      <c r="F47" t="s">
-        <v>73</v>
-      </c>
       <c r="I47" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -1932,8 +2018,11 @@
       <c r="I48" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -1955,8 +2044,11 @@
       <c r="I49" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1972,17 +2064,17 @@
       <c r="E50" t="s">
         <v>73</v>
       </c>
-      <c r="F50" t="s">
-        <v>73</v>
-      </c>
       <c r="H50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I50" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2002,7 +2094,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -2018,11 +2110,11 @@
       <c r="E52" t="s">
         <v>73</v>
       </c>
-      <c r="F52" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I52" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>27</v>
       </c>
@@ -2038,7 +2130,7 @@
       <c r="E53" t="s">
         <v>97</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G53" t="s">
@@ -2050,8 +2142,11 @@
       <c r="I53" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -2067,11 +2162,8 @@
       <c r="E54" t="s">
         <v>73</v>
       </c>
-      <c r="F54" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>32</v>
       </c>
@@ -2087,11 +2179,11 @@
       <c r="E55" t="s">
         <v>73</v>
       </c>
-      <c r="F55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -2108,7 +2200,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -2125,7 +2217,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -2141,7 +2233,7 @@
       <c r="E58" t="s">
         <v>73</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G58" t="s">
@@ -2153,8 +2245,11 @@
       <c r="I58" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -2171,7 +2266,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -2188,7 +2283,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -2205,7 +2300,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -2228,7 +2323,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2244,11 +2339,8 @@
       <c r="E63" t="s">
         <v>73</v>
       </c>
-      <c r="F63" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -2270,8 +2362,11 @@
       <c r="I64" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J64" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -2287,7 +2382,7 @@
       <c r="E65" t="s">
         <v>96</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="2" t="s">
         <v>73</v>
       </c>
       <c r="H65" t="s">
@@ -2296,8 +2391,11 @@
       <c r="I65" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J65" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -2313,7 +2411,7 @@
       <c r="E66" t="s">
         <v>97</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G66" t="s">
@@ -2322,8 +2420,11 @@
       <c r="I66" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J66" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>21</v>
       </c>
@@ -2345,13 +2446,12 @@
       <c r="I67" t="s">
         <v>73</v>
       </c>
+      <c r="J67" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I67">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:J67" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
added transposed correlations plot, added correlations back to cohort_overview_table
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC847A30-43E6-4318-9403-32E6CD836BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7B4443-C2E4-4405-88EB-60009A9A1CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="111">
   <si>
     <t>row_id</t>
   </si>
@@ -815,8 +815,8 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,6 +881,9 @@
       <c r="E2" t="s">
         <v>73</v>
       </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
       <c r="I2" t="s">
         <v>73</v>
       </c>
@@ -904,6 +907,9 @@
       <c r="E3" t="s">
         <v>73</v>
       </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
       <c r="I3" t="s">
         <v>73</v>
       </c>
@@ -934,6 +940,7 @@
       <c r="H4" t="s">
         <v>74</v>
       </c>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -951,6 +958,9 @@
       <c r="E5" t="s">
         <v>73</v>
       </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
       <c r="I5" t="s">
         <v>73</v>
       </c>
@@ -1071,6 +1081,9 @@
       <c r="E11" t="s">
         <v>73</v>
       </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
       <c r="I11" t="s">
         <v>73</v>
       </c>
@@ -1103,7 +1116,7 @@
       <c r="I12" t="s">
         <v>73</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1149,6 +1162,9 @@
       <c r="E14" t="s">
         <v>73</v>
       </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
       <c r="I14" t="s">
         <v>73</v>
       </c>
@@ -1184,7 +1200,7 @@
       <c r="I15" t="s">
         <v>73</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1213,7 +1229,7 @@
       <c r="I16" t="s">
         <v>73</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1239,7 +1255,7 @@
       <c r="I17" t="s">
         <v>73</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1265,7 +1281,7 @@
       <c r="I18" t="s">
         <v>73</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1291,7 +1307,7 @@
       <c r="I19" t="s">
         <v>73</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1317,7 +1333,7 @@
       <c r="I20" t="s">
         <v>73</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1346,7 +1362,7 @@
       <c r="I21" t="s">
         <v>73</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1398,7 +1414,7 @@
       <c r="I23" t="s">
         <v>73</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1425,6 +1441,7 @@
       <c r="H24" t="s">
         <v>104</v>
       </c>
+      <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1454,7 +1471,7 @@
       <c r="I25" t="s">
         <v>73</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1486,7 +1503,7 @@
       <c r="I26" t="s">
         <v>73</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1506,6 +1523,9 @@
       <c r="E27" t="s">
         <v>73</v>
       </c>
+      <c r="F27" t="s">
+        <v>73</v>
+      </c>
       <c r="I27" t="s">
         <v>73</v>
       </c>
@@ -1529,6 +1549,9 @@
       <c r="E28" t="s">
         <v>73</v>
       </c>
+      <c r="F28" t="s">
+        <v>73</v>
+      </c>
       <c r="I28" t="s">
         <v>73</v>
       </c>
@@ -1615,6 +1638,9 @@
       <c r="E32" t="s">
         <v>73</v>
       </c>
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
       <c r="I32" t="s">
         <v>73</v>
       </c>
@@ -1673,7 +1699,7 @@
       <c r="I34" t="s">
         <v>73</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J34" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1736,6 +1762,9 @@
       <c r="E37" t="s">
         <v>73</v>
       </c>
+      <c r="F37" t="s">
+        <v>73</v>
+      </c>
       <c r="I37" t="s">
         <v>73</v>
       </c>
@@ -1763,6 +1792,7 @@
       <c r="H38" t="s">
         <v>76</v>
       </c>
+      <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -1789,7 +1819,7 @@
       <c r="I39" t="s">
         <v>73</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1821,7 +1851,7 @@
       <c r="I40" t="s">
         <v>73</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1853,7 +1883,7 @@
       <c r="I41" t="s">
         <v>73</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1873,9 +1903,6 @@
       <c r="E42" t="s">
         <v>73</v>
       </c>
-      <c r="F42" t="s">
-        <v>73</v>
-      </c>
       <c r="H42" t="s">
         <v>90</v>
       </c>
@@ -1925,7 +1952,7 @@
       <c r="I44" t="s">
         <v>73</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1952,6 +1979,7 @@
       <c r="H45" t="s">
         <v>104</v>
       </c>
+      <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -1989,6 +2017,9 @@
       <c r="E47" t="s">
         <v>73</v>
       </c>
+      <c r="F47" t="s">
+        <v>73</v>
+      </c>
       <c r="I47" t="s">
         <v>73</v>
       </c>
@@ -2064,6 +2095,9 @@
       <c r="E50" t="s">
         <v>73</v>
       </c>
+      <c r="F50" t="s">
+        <v>73</v>
+      </c>
       <c r="H50" t="s">
         <v>106</v>
       </c>
@@ -2110,6 +2144,9 @@
       <c r="E52" t="s">
         <v>73</v>
       </c>
+      <c r="F52" t="s">
+        <v>73</v>
+      </c>
       <c r="I52" t="s">
         <v>73</v>
       </c>
@@ -2142,7 +2179,7 @@
       <c r="I53" t="s">
         <v>73</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J53" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2245,7 +2282,7 @@
       <c r="I58" t="s">
         <v>73</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J58" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2339,6 +2376,9 @@
       <c r="E63" t="s">
         <v>73</v>
       </c>
+      <c r="F63" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
@@ -2391,7 +2431,7 @@
       <c r="I65" t="s">
         <v>73</v>
       </c>
-      <c r="J65" t="s">
+      <c r="J65" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2420,7 +2460,7 @@
       <c r="I66" t="s">
         <v>73</v>
       </c>
-      <c r="J66" t="s">
+      <c r="J66" s="2" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added one-hot-encoding to pacmap and clustering, cleanup
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBF99C1-C0E5-4F8E-8624-FA4B41C94A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1574B30E-0BD8-418B-B67F-46485B3E3CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="113">
   <si>
     <t>row_id</t>
   </si>
@@ -821,8 +821,8 @@
   <dimension ref="A1:K67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1017,9 +1017,6 @@
       <c r="E7" t="s">
         <v>73</v>
       </c>
-      <c r="F7" t="s">
-        <v>73</v>
-      </c>
       <c r="H7" t="s">
         <v>112</v>
       </c>
@@ -1106,9 +1103,6 @@
       <c r="E11" t="s">
         <v>73</v>
       </c>
-      <c r="F11" t="s">
-        <v>73</v>
-      </c>
       <c r="I11" t="s">
         <v>73</v>
       </c>
@@ -1588,9 +1582,6 @@
       <c r="E27" t="s">
         <v>73</v>
       </c>
-      <c r="F27" t="s">
-        <v>73</v>
-      </c>
       <c r="I27" t="s">
         <v>73</v>
       </c>
@@ -1718,9 +1709,6 @@
       <c r="E32" t="s">
         <v>73</v>
       </c>
-      <c r="F32" t="s">
-        <v>73</v>
-      </c>
       <c r="I32" t="s">
         <v>73</v>
       </c>
@@ -2022,9 +2010,6 @@
       <c r="E43" t="s">
         <v>73</v>
       </c>
-      <c r="F43" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
@@ -2123,9 +2108,6 @@
       <c r="E47" t="s">
         <v>73</v>
       </c>
-      <c r="F47" t="s">
-        <v>73</v>
-      </c>
       <c r="I47" t="s">
         <v>73</v>
       </c>
@@ -2441,9 +2423,6 @@
         <v>89</v>
       </c>
       <c r="E60" t="s">
-        <v>73</v>
-      </c>
-      <c r="F60" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added fairness metrics first draft
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C065535D-CF3B-402A-994B-F960B9D0FD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171E42A4-349C-4A35-AF33-D02A8285E076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="116">
   <si>
     <t>row_id</t>
   </si>
@@ -497,10 +497,34 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -509,10 +533,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -831,7 +858,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M53" sqref="M53"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -841,7 +868,7 @@
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="9.77734375" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" customWidth="1"/>
     <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
@@ -867,7 +894,7 @@
       <c r="E1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -937,7 +964,7 @@
       <c r="E3" t="s">
         <v>73</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I3" t="s">
@@ -975,7 +1002,7 @@
       <c r="E4" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="5"/>
       <c r="G4" t="s">
         <v>73</v>
       </c>
@@ -1003,7 +1030,7 @@
       <c r="E5" t="s">
         <v>73</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I5" t="s">
@@ -1098,7 +1125,7 @@
       <c r="E9" t="s">
         <v>73</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I9" t="s">
@@ -1173,7 +1200,7 @@
       <c r="E12" t="s">
         <v>97</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G12" t="s">
@@ -1214,7 +1241,7 @@
       <c r="E13" t="s">
         <v>73</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I13" t="s">
@@ -1252,7 +1279,7 @@
       <c r="E14" t="s">
         <v>73</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I14" t="s">
@@ -1290,7 +1317,7 @@
       <c r="E15" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G15" t="s">
@@ -1331,7 +1358,7 @@
       <c r="E16" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="5" t="s">
         <v>73</v>
       </c>
       <c r="H16" t="s">
@@ -1372,7 +1399,7 @@
       <c r="E17" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="5" t="s">
         <v>73</v>
       </c>
       <c r="I17" t="s">
@@ -1407,7 +1434,7 @@
       <c r="E18" t="s">
         <v>103</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="5" t="s">
         <v>73</v>
       </c>
       <c r="I18" t="s">
@@ -1442,7 +1469,7 @@
       <c r="E19" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="5" t="s">
         <v>73</v>
       </c>
       <c r="I19" t="s">
@@ -1477,7 +1504,7 @@
       <c r="E20" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="5" t="s">
         <v>73</v>
       </c>
       <c r="I20" t="s">
@@ -1512,7 +1539,7 @@
       <c r="E21" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="5" t="s">
         <v>73</v>
       </c>
       <c r="H21" t="s">
@@ -1570,7 +1597,7 @@
       <c r="E23" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G23" t="s">
@@ -1611,7 +1638,7 @@
       <c r="E24" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="5"/>
       <c r="G24" t="s">
         <v>73</v>
       </c>
@@ -1639,7 +1666,7 @@
       <c r="E25" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G25" t="s">
@@ -1680,7 +1707,7 @@
       <c r="E26" t="s">
         <v>84</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G26" t="s">
@@ -1721,7 +1748,7 @@
       <c r="E27" t="s">
         <v>73</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I27" t="s">
@@ -1756,7 +1783,7 @@
       <c r="E28" t="s">
         <v>73</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I28" t="s">
@@ -1837,7 +1864,7 @@
       <c r="E31" t="s">
         <v>73</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I31" t="s">
@@ -1875,6 +1902,9 @@
       <c r="E32" t="s">
         <v>73</v>
       </c>
+      <c r="F32" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="I32" t="s">
         <v>73</v>
       </c>
@@ -1882,6 +1912,9 @@
         <v>73</v>
       </c>
       <c r="K32" t="s">
+        <v>73</v>
+      </c>
+      <c r="L32" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1901,7 +1934,7 @@
       <c r="E33" t="s">
         <v>73</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I33" t="s">
@@ -1911,9 +1944,6 @@
         <v>73</v>
       </c>
       <c r="K33" t="s">
-        <v>73</v>
-      </c>
-      <c r="L33" t="s">
         <v>73</v>
       </c>
       <c r="M33" t="s">
@@ -1939,7 +1969,7 @@
       <c r="E34" t="s">
         <v>97</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G34" t="s">
@@ -1977,7 +2007,7 @@
       <c r="E35" t="s">
         <v>73</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I35" t="s">
@@ -2052,7 +2082,7 @@
       <c r="E38" t="s">
         <v>97</v>
       </c>
-      <c r="F38" s="2"/>
+      <c r="F38" s="5"/>
       <c r="G38" t="s">
         <v>73</v>
       </c>
@@ -2080,7 +2110,7 @@
       <c r="E39" t="s">
         <v>98</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="5" t="s">
         <v>73</v>
       </c>
       <c r="H39" t="s">
@@ -2118,7 +2148,7 @@
       <c r="E40" t="s">
         <v>73</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G40" t="s">
@@ -2159,7 +2189,7 @@
       <c r="E41" t="s">
         <v>96</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G41" t="s">
@@ -2237,7 +2267,7 @@
       <c r="E44" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G44" t="s">
@@ -2278,7 +2308,7 @@
       <c r="E45" t="s">
         <v>73</v>
       </c>
-      <c r="F45" s="2"/>
+      <c r="F45" s="5"/>
       <c r="G45" t="s">
         <v>73</v>
       </c>
@@ -2352,7 +2382,7 @@
       <c r="E48" t="s">
         <v>73</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I48" t="s">
@@ -2390,7 +2420,7 @@
       <c r="E49" t="s">
         <v>73</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I49" t="s">
@@ -2428,7 +2458,7 @@
       <c r="E50" t="s">
         <v>73</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H50" t="s">
@@ -2509,7 +2539,7 @@
       <c r="E53" t="s">
         <v>97</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F53" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G53" t="s">
@@ -2624,7 +2654,7 @@
       <c r="E58" t="s">
         <v>73</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F58" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G58" t="s">
@@ -2756,7 +2786,7 @@
       <c r="E64" t="s">
         <v>73</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I64" t="s">
@@ -2794,7 +2824,7 @@
       <c r="E65" t="s">
         <v>96</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F65" s="5" t="s">
         <v>73</v>
       </c>
       <c r="H65" t="s">
@@ -2835,7 +2865,7 @@
       <c r="E66" t="s">
         <v>97</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F66" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G66" t="s">
@@ -2873,7 +2903,7 @@
       <c r="E67" t="s">
         <v>73</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I67" t="s">

</xml_diff>

<commit_message>
first draft for plot_performance_metrics()
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanek\Documents\Programmieren\Python\PyCharm\MA_thesis\supplements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2DFA54-64DF-4615-A463-454EE601D657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA26D91B-1CCC-4548-96D6-000F57607FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="116">
   <si>
     <t>row_id</t>
   </si>
@@ -857,28 +857,28 @@
   <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="20.54296875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" customWidth="1"/>
-    <col min="8" max="8" width="18.6328125" customWidth="1"/>
-    <col min="9" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
@@ -922,7 +922,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -948,7 +948,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -986,7 +986,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1014,7 +1014,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1650,7 +1650,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -2097,7 +2097,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -2253,8 +2253,11 @@
       <c r="E43" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F43" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -2295,7 +2298,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -2323,7 +2326,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -2343,7 +2346,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -2359,6 +2362,9 @@
       <c r="E47" t="s">
         <v>73</v>
       </c>
+      <c r="F47" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="I47" t="s">
         <v>73</v>
       </c>
@@ -2369,7 +2375,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2407,7 +2413,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -2445,7 +2451,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2486,7 +2492,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2506,7 +2512,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -2526,7 +2532,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>27</v>
       </c>
@@ -2567,7 +2573,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -2584,7 +2590,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>32</v>
       </c>
@@ -2607,7 +2613,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -2624,7 +2630,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -2641,7 +2647,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -2682,7 +2688,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -2699,7 +2705,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -2715,8 +2721,11 @@
       <c r="E60" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F60" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -2733,7 +2742,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -2756,7 +2765,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2773,7 +2782,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -2811,7 +2820,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -2852,7 +2861,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -2890,7 +2899,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
finished deep learning model
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanek\Documents\Programmieren\Python\PyCharm\MA_thesis\supplements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57367DF1-D4DF-4128-A258-9FFEEE183845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DF1119-E09B-4E35-B520-CA55E661DA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="115">
   <si>
     <t>row_id</t>
   </si>
@@ -854,28 +854,29 @@
   <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="20.54296875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" customWidth="1"/>
-    <col min="8" max="8" width="18.6328125" customWidth="1"/>
-    <col min="9" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" customWidth="1"/>
+    <col min="14" max="14" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
@@ -919,7 +920,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -935,6 +936,9 @@
       <c r="E2" t="s">
         <v>73</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="I2" t="s">
         <v>73</v>
       </c>
@@ -945,7 +949,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -983,7 +987,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1011,7 +1015,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1049,7 +1053,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1066,7 +1070,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1089,7 +1093,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1106,7 +1110,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1144,7 +1148,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1161,7 +1165,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1181,7 +1185,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1197,9 +1201,7 @@
       <c r="E12" t="s">
         <v>97</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="F12" s="5"/>
       <c r="G12" t="s">
         <v>73</v>
       </c>
@@ -1222,7 +1224,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1260,7 +1262,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1298,7 +1300,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1314,9 +1316,7 @@
       <c r="E15" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="F15" s="5"/>
       <c r="G15" t="s">
         <v>73</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -1355,7 +1355,7 @@
       <c r="E16" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="2" t="s">
         <v>73</v>
       </c>
       <c r="H16" t="s">
@@ -1380,7 +1380,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1396,7 +1396,7 @@
       <c r="E17" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I17" t="s">
@@ -1415,7 +1415,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1431,7 +1431,7 @@
       <c r="E18" t="s">
         <v>103</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I18" t="s">
@@ -1450,7 +1450,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1466,7 +1466,7 @@
       <c r="E19" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I19" t="s">
@@ -1485,7 +1485,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1501,7 +1501,7 @@
       <c r="E20" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I20" t="s">
@@ -1520,7 +1520,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1536,7 +1536,7 @@
       <c r="E21" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="2" t="s">
         <v>73</v>
       </c>
       <c r="H21" t="s">
@@ -1558,7 +1558,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1574,14 +1574,11 @@
       <c r="E22" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="I22" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1597,7 +1594,7 @@
       <c r="E23" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G23" t="s">
@@ -1622,7 +1619,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1638,7 +1635,7 @@
       <c r="E24" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="2"/>
       <c r="G24" t="s">
         <v>73</v>
       </c>
@@ -1650,7 +1647,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1666,7 +1663,7 @@
       <c r="E25" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G25" t="s">
@@ -1691,7 +1688,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1707,7 +1704,7 @@
       <c r="E26" t="s">
         <v>84</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G26" t="s">
@@ -1732,7 +1729,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1748,9 +1745,6 @@
       <c r="E27" t="s">
         <v>73</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="I27" t="s">
         <v>73</v>
       </c>
@@ -1767,7 +1761,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1805,7 +1799,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1828,7 +1822,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1851,7 +1845,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1889,7 +1883,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1921,7 +1915,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1937,9 +1931,6 @@
       <c r="E33" t="s">
         <v>73</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="I33" t="s">
         <v>73</v>
       </c>
@@ -1956,7 +1947,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -1994,7 +1985,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2032,7 +2023,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -2049,7 +2040,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -2065,14 +2056,11 @@
       <c r="E37" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="I37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -2088,7 +2076,7 @@
       <c r="E38" t="s">
         <v>97</v>
       </c>
-      <c r="F38" s="5"/>
+      <c r="F38" s="2"/>
       <c r="G38" t="s">
         <v>73</v>
       </c>
@@ -2100,7 +2088,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -2116,7 +2104,7 @@
       <c r="E39" t="s">
         <v>98</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="2" t="s">
         <v>73</v>
       </c>
       <c r="H39" t="s">
@@ -2138,7 +2126,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -2154,7 +2142,7 @@
       <c r="E40" t="s">
         <v>73</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G40" t="s">
@@ -2179,7 +2167,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -2195,7 +2183,7 @@
       <c r="E41" t="s">
         <v>96</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G41" t="s">
@@ -2220,7 +2208,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2240,7 +2228,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -2256,11 +2244,8 @@
       <c r="E43" t="s">
         <v>73</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -2276,7 +2261,7 @@
       <c r="E44" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G44" t="s">
@@ -2301,7 +2286,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -2329,7 +2314,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -2349,7 +2334,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -2365,9 +2350,6 @@
       <c r="E47" t="s">
         <v>73</v>
       </c>
-      <c r="F47" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="I47" t="s">
         <v>73</v>
       </c>
@@ -2378,7 +2360,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2416,7 +2398,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -2454,7 +2436,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2495,7 +2477,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2515,7 +2497,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -2531,14 +2513,11 @@
       <c r="E52" t="s">
         <v>73</v>
       </c>
-      <c r="F52" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="I52" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>27</v>
       </c>
@@ -2579,7 +2558,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -2596,7 +2575,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>32</v>
       </c>
@@ -2612,14 +2591,11 @@
       <c r="E55" t="s">
         <v>73</v>
       </c>
-      <c r="F55" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="J55" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -2636,7 +2612,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -2653,7 +2629,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -2694,7 +2670,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -2711,7 +2687,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -2727,11 +2703,8 @@
       <c r="E60" t="s">
         <v>73</v>
       </c>
-      <c r="F60" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -2748,7 +2721,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -2771,7 +2744,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2787,11 +2760,8 @@
       <c r="E63" t="s">
         <v>73</v>
       </c>
-      <c r="F63" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -2829,7 +2799,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -2870,7 +2840,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -2908,7 +2878,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
added deep learning model to model comparison pipeline
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DF1119-E09B-4E35-B520-CA55E661DA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD36FC9-EBE8-4F7C-95F5-5D0DB6FD6E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="115">
   <si>
     <t>row_id</t>
   </si>
@@ -854,8 +854,8 @@
   <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2452,9 +2452,6 @@
       <c r="E50" t="s">
         <v>73</v>
       </c>
-      <c r="F50" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="H50" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
created output for overleaf
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D5B003-F483-42BE-B180-0D947978ED04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DF7B5E-94E2-4397-A024-F27087B863FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -851,11 +851,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -987,7 +988,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1053,7 +1054,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1070,7 +1071,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1093,7 +1094,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1148,7 +1149,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1165,7 +1166,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1185,7 +1186,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1300,7 +1301,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1573,7 +1574,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1634,7 +1635,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1744,7 +1745,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1837,7 +1838,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1930,7 +1931,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2038,7 +2039,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -2075,7 +2076,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -2223,7 +2224,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2243,7 +2244,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -2301,7 +2302,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -2329,7 +2330,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -2349,7 +2350,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -2492,7 +2493,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2512,7 +2513,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -2573,7 +2574,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -2590,7 +2591,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>32</v>
       </c>
@@ -2610,7 +2611,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -2627,7 +2628,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -2685,7 +2686,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -2702,7 +2703,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -2719,7 +2720,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -2736,7 +2737,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -2759,7 +2760,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2932,7 +2933,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N67" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}"/>
+  <autoFilter ref="A1:N67" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
+    <filterColumn colId="5">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
added further relevant features to analysis and frontend
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DF7B5E-94E2-4397-A024-F27087B863FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE9DA60-827B-4C32-B520-0A259FFE5896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="115">
   <si>
     <t>row_id</t>
   </si>
@@ -851,12 +851,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,7 +987,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1054,7 +1053,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1087,6 +1086,9 @@
       <c r="E7" t="s">
         <v>73</v>
       </c>
+      <c r="F7" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="H7" t="s">
         <v>111</v>
       </c>
@@ -1094,7 +1096,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1149,7 +1151,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1166,7 +1168,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1182,11 +1184,14 @@
       <c r="E11" t="s">
         <v>73</v>
       </c>
+      <c r="F11" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="I11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1301,7 +1306,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1574,7 +1579,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1635,7 +1640,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1745,7 +1750,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1759,6 +1764,9 @@
         <v>89</v>
       </c>
       <c r="E27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I27" t="s">
@@ -1838,7 +1846,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1931,7 +1939,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1945,6 +1953,9 @@
         <v>88</v>
       </c>
       <c r="E33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I33" t="s">
@@ -2039,7 +2050,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -2056,7 +2067,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -2072,11 +2083,14 @@
       <c r="E37" t="s">
         <v>73</v>
       </c>
+      <c r="F37" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="I37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -2224,7 +2238,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2244,7 +2258,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -2258,6 +2272,9 @@
         <v>89</v>
       </c>
       <c r="E43" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2302,7 +2319,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -2330,7 +2347,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -2350,7 +2367,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -2364,6 +2381,9 @@
         <v>89</v>
       </c>
       <c r="E47" t="s">
+        <v>73</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I47" t="s">
@@ -2493,7 +2513,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2513,7 +2533,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -2574,7 +2594,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -2591,7 +2611,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>32</v>
       </c>
@@ -2607,11 +2627,14 @@
       <c r="E55" t="s">
         <v>73</v>
       </c>
+      <c r="F55" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="J55" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -2628,7 +2651,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -2686,7 +2709,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -2703,7 +2726,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -2719,8 +2742,11 @@
       <c r="E60" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F60" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -2736,8 +2762,11 @@
       <c r="E61" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F61" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -2760,7 +2789,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2933,13 +2962,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N67" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
-    <filterColumn colId="5">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N67" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
improved fairness metrics table, also title for DL plot in one line
</commit_message>
<xml_diff>
--- a/supplements/feature_preprocessing_table.xlsx
+++ b/supplements/feature_preprocessing_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE9DA60-827B-4C32-B520-0A259FFE5896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B85F640-47F5-4560-8ADC-7B4940924071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{16A02474-CB70-4690-90AB-ECD68D89D2CE}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$N$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$P$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="117">
   <si>
     <t>row_id</t>
   </si>
@@ -444,6 +444,12 @@
   </si>
   <si>
     <t>selection_clustering_curr</t>
+  </si>
+  <si>
+    <t>optimized_selection</t>
+  </si>
+  <si>
+    <t>standard_selection</t>
   </si>
 </sst>
 </file>
@@ -480,7 +486,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,6 +496,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -530,13 +542,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -851,36 +866,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}">
-  <dimension ref="A1:N67"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.21875" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" style="3" customWidth="1"/>
+    <col min="7" max="8" width="20.5546875" style="6" customWidth="1"/>
     <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.88671875" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" customWidth="1"/>
-    <col min="14" max="14" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.88671875" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" customWidth="1"/>
+    <col min="16" max="16" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -892,35 +908,41 @@
       <c r="E1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -936,20 +958,24 @@
       <c r="E2" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="F2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="K2" t="s">
         <v>73</v>
       </c>
       <c r="L2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -965,15 +991,13 @@
       <c r="E3" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" t="s">
-        <v>73</v>
-      </c>
+      <c r="F3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="3"/>
       <c r="K3" t="s">
         <v>73</v>
       </c>
@@ -986,8 +1010,14 @@
       <c r="N3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" t="s">
+        <v>73</v>
+      </c>
+      <c r="P3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1003,19 +1033,21 @@
       <c r="E4" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1031,13 +1063,13 @@
       <c r="E5" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="F5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>73</v>
       </c>
       <c r="K5" t="s">
@@ -1052,8 +1084,14 @@
       <c r="N5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5" t="s">
+        <v>73</v>
+      </c>
+      <c r="P5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1069,8 +1107,10 @@
       <c r="E6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1086,17 +1126,21 @@
       <c r="E7" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="F7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="J7" t="s">
         <v>111</v>
       </c>
-      <c r="I7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1112,8 +1156,10 @@
       <c r="E8" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1129,15 +1175,13 @@
       <c r="E9" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I9" t="s">
-        <v>73</v>
-      </c>
-      <c r="J9" t="s">
-        <v>73</v>
-      </c>
+      <c r="F9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="3"/>
       <c r="K9" t="s">
         <v>73</v>
       </c>
@@ -1150,8 +1194,14 @@
       <c r="N9" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O9" t="s">
+        <v>73</v>
+      </c>
+      <c r="P9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1167,8 +1217,10 @@
       <c r="E10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1184,14 +1236,18 @@
       <c r="E11" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="K11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1207,30 +1263,32 @@
       <c r="E12" t="s">
         <v>97</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" t="s">
-        <v>73</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" t="s">
         <v>101</v>
       </c>
-      <c r="I12" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N12" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1246,15 +1304,13 @@
       <c r="E13" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I13" t="s">
-        <v>73</v>
-      </c>
-      <c r="J13" t="s">
-        <v>73</v>
-      </c>
+      <c r="F13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="3"/>
       <c r="K13" t="s">
         <v>73</v>
       </c>
@@ -1267,8 +1323,14 @@
       <c r="N13" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O13" t="s">
+        <v>73</v>
+      </c>
+      <c r="P13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1284,15 +1346,13 @@
       <c r="E14" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" t="s">
-        <v>73</v>
-      </c>
-      <c r="J14" t="s">
-        <v>73</v>
-      </c>
+      <c r="F14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="3"/>
       <c r="K14" t="s">
         <v>73</v>
       </c>
@@ -1305,8 +1365,14 @@
       <c r="N14" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>73</v>
+      </c>
+      <c r="P14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1322,30 +1388,32 @@
       <c r="E15" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" t="s">
         <v>104</v>
       </c>
-      <c r="I15" t="s">
-        <v>73</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" t="s">
+        <v>73</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N15" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -1364,29 +1432,35 @@
       <c r="F16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H16" t="s">
+      <c r="G16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" t="s">
         <v>99</v>
       </c>
-      <c r="I16" t="s">
-        <v>73</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="K16" t="s">
+        <v>73</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N16" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N16" t="s">
+        <v>73</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1405,26 +1479,32 @@
       <c r="F17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I17" t="s">
-        <v>73</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="G17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K17" t="s">
+        <v>73</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N17" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N17" t="s">
+        <v>73</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1443,26 +1523,32 @@
       <c r="F18" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I18" t="s">
-        <v>73</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="G18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K18" t="s">
+        <v>73</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N18" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N18" t="s">
+        <v>73</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1481,26 +1567,32 @@
       <c r="F19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I19" t="s">
-        <v>73</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L19" t="s">
+      <c r="G19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K19" t="s">
+        <v>73</v>
+      </c>
+      <c r="L19" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N19" t="s">
+        <v>73</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1519,26 +1611,32 @@
       <c r="F20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I20" t="s">
-        <v>73</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="G20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K20" t="s">
+        <v>73</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N20" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N20" t="s">
+        <v>73</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1557,29 +1655,35 @@
       <c r="F21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H21" t="s">
+      <c r="G21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J21" t="s">
         <v>86</v>
       </c>
-      <c r="I21" t="s">
-        <v>73</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="K21" t="s">
+        <v>73</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N21" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N21" t="s">
+        <v>73</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1595,11 +1699,13 @@
       <c r="E22" t="s">
         <v>73</v>
       </c>
-      <c r="I22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="K22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1618,29 +1724,35 @@
       <c r="F23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G23" t="s">
-        <v>73</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="G23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" t="s">
+        <v>73</v>
+      </c>
+      <c r="J23" t="s">
         <v>74</v>
       </c>
-      <c r="I23" t="s">
-        <v>73</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K23" s="2" t="s">
+      <c r="K23" t="s">
+        <v>73</v>
+      </c>
+      <c r="L23" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N23" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1657,18 +1769,20 @@
         <v>73</v>
       </c>
       <c r="F24" s="2"/>
-      <c r="G24" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" t="s">
+        <v>73</v>
+      </c>
+      <c r="J24" t="s">
         <v>104</v>
       </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1687,29 +1801,35 @@
       <c r="F25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G25" t="s">
-        <v>73</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="G25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J25" t="s">
         <v>101</v>
       </c>
-      <c r="I25" t="s">
-        <v>73</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K25" s="2" t="s">
+      <c r="K25" t="s">
+        <v>73</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N25" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1728,29 +1848,35 @@
       <c r="F26" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G26" t="s">
-        <v>73</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="G26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" t="s">
+        <v>73</v>
+      </c>
+      <c r="J26" t="s">
         <v>101</v>
       </c>
-      <c r="I26" t="s">
-        <v>73</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K26" s="2" t="s">
+      <c r="K26" t="s">
+        <v>73</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N26" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1766,26 +1892,30 @@
       <c r="E27" t="s">
         <v>73</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I27" t="s">
-        <v>73</v>
-      </c>
-      <c r="J27" t="s">
-        <v>73</v>
-      </c>
+      <c r="F27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" s="3"/>
       <c r="K27" t="s">
         <v>73</v>
       </c>
+      <c r="L27" t="s">
+        <v>73</v>
+      </c>
       <c r="M27" t="s">
         <v>73</v>
       </c>
-      <c r="N27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O27" t="s">
+        <v>73</v>
+      </c>
+      <c r="P27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1801,15 +1931,13 @@
       <c r="E28" t="s">
         <v>73</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I28" t="s">
-        <v>73</v>
-      </c>
-      <c r="J28" t="s">
-        <v>73</v>
-      </c>
+      <c r="F28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" s="3"/>
       <c r="K28" t="s">
         <v>73</v>
       </c>
@@ -1822,8 +1950,14 @@
       <c r="N28" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O28" t="s">
+        <v>73</v>
+      </c>
+      <c r="P28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1839,14 +1973,20 @@
       <c r="E29" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="L29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F29" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="N29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1862,14 +2002,16 @@
       <c r="E30" t="s">
         <v>73</v>
       </c>
-      <c r="I30" t="s">
-        <v>73</v>
-      </c>
-      <c r="J30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="K30" t="s">
+        <v>73</v>
+      </c>
+      <c r="L30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1885,13 +2027,13 @@
       <c r="E31" t="s">
         <v>73</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I31" t="s">
-        <v>73</v>
-      </c>
-      <c r="J31" t="s">
+      <c r="F31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>73</v>
       </c>
       <c r="K31" t="s">
@@ -1906,8 +2048,14 @@
       <c r="N31" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O31" t="s">
+        <v>73</v>
+      </c>
+      <c r="P31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1923,13 +2071,13 @@
       <c r="E32" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I32" t="s">
-        <v>73</v>
-      </c>
-      <c r="J32" t="s">
+      <c r="F32" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" s="3" t="s">
         <v>73</v>
       </c>
       <c r="K32" t="s">
@@ -1938,8 +2086,14 @@
       <c r="L32" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M32" t="s">
+        <v>73</v>
+      </c>
+      <c r="N32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1955,26 +2109,30 @@
       <c r="E33" t="s">
         <v>73</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I33" t="s">
-        <v>73</v>
-      </c>
-      <c r="J33" t="s">
-        <v>73</v>
-      </c>
+      <c r="F33" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H33" s="3"/>
       <c r="K33" t="s">
         <v>73</v>
       </c>
+      <c r="L33" t="s">
+        <v>73</v>
+      </c>
       <c r="M33" t="s">
         <v>73</v>
       </c>
-      <c r="N33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O33" t="s">
+        <v>73</v>
+      </c>
+      <c r="P33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -1990,29 +2148,35 @@
       <c r="E34" t="s">
         <v>97</v>
       </c>
-      <c r="F34" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="F34" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I34" t="s">
         <v>73</v>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K34" s="2" t="s">
+      <c r="K34" t="s">
+        <v>73</v>
+      </c>
+      <c r="L34" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N34" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2028,13 +2192,13 @@
       <c r="E35" t="s">
         <v>73</v>
       </c>
-      <c r="F35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I35" t="s">
-        <v>73</v>
-      </c>
-      <c r="J35" t="s">
+      <c r="F35" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>73</v>
       </c>
       <c r="K35" t="s">
@@ -2049,8 +2213,14 @@
       <c r="N35" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O35" t="s">
+        <v>73</v>
+      </c>
+      <c r="P35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -2066,8 +2236,10 @@
       <c r="E36" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -2083,14 +2255,18 @@
       <c r="E37" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F37" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H37" s="3"/>
+      <c r="K37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -2107,18 +2283,20 @@
         <v>97</v>
       </c>
       <c r="F38" s="2"/>
-      <c r="G38" t="s">
-        <v>73</v>
-      </c>
-      <c r="H38" t="s">
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" t="s">
+        <v>73</v>
+      </c>
+      <c r="J38" t="s">
         <v>76</v>
       </c>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
       <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -2137,26 +2315,32 @@
       <c r="F39" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H39" t="s">
+      <c r="G39" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J39" t="s">
         <v>105</v>
       </c>
-      <c r="I39" t="s">
-        <v>73</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K39" s="2" t="s">
+      <c r="K39" t="s">
+        <v>73</v>
+      </c>
+      <c r="L39" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N39" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O39" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -2175,29 +2359,35 @@
       <c r="F40" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G40" t="s">
-        <v>73</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="G40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" t="s">
+        <v>73</v>
+      </c>
+      <c r="J40" t="s">
         <v>104</v>
       </c>
-      <c r="I40" t="s">
-        <v>73</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K40" s="2" t="s">
+      <c r="K40" t="s">
+        <v>73</v>
+      </c>
+      <c r="L40" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N40" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -2216,29 +2406,35 @@
       <c r="F41" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G41" t="s">
-        <v>73</v>
-      </c>
-      <c r="H41" t="s">
+      <c r="G41" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I41" t="s">
+        <v>73</v>
+      </c>
+      <c r="J41" t="s">
         <v>93</v>
       </c>
-      <c r="I41" t="s">
-        <v>73</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K41" s="2" t="s">
+      <c r="K41" t="s">
+        <v>73</v>
+      </c>
+      <c r="L41" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N41" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O41" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2254,11 +2450,13 @@
       <c r="E42" t="s">
         <v>73</v>
       </c>
-      <c r="H42" t="s">
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="J42" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -2274,11 +2472,15 @@
       <c r="E43" t="s">
         <v>73</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F43" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -2297,29 +2499,35 @@
       <c r="F44" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G44" t="s">
-        <v>73</v>
-      </c>
-      <c r="H44" t="s">
+      <c r="G44" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I44" t="s">
+        <v>73</v>
+      </c>
+      <c r="J44" t="s">
         <v>101</v>
       </c>
-      <c r="I44" t="s">
-        <v>73</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K44" s="2" t="s">
+      <c r="K44" t="s">
+        <v>73</v>
+      </c>
+      <c r="L44" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N44" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O44" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -2335,19 +2543,21 @@
       <c r="E45" t="s">
         <v>73</v>
       </c>
-      <c r="F45" s="5"/>
-      <c r="G45" t="s">
-        <v>73</v>
-      </c>
-      <c r="H45" t="s">
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" t="s">
+        <v>73</v>
+      </c>
+      <c r="J45" t="s">
         <v>104</v>
       </c>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
       <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -2363,11 +2573,13 @@
       <c r="E46" t="s">
         <v>73</v>
       </c>
-      <c r="H46" t="s">
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="J46" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -2383,20 +2595,24 @@
       <c r="E47" t="s">
         <v>73</v>
       </c>
-      <c r="F47" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I47" t="s">
-        <v>73</v>
-      </c>
-      <c r="J47" t="s">
-        <v>73</v>
-      </c>
+      <c r="F47" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H47" s="3"/>
       <c r="K47" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L47" t="s">
+        <v>73</v>
+      </c>
+      <c r="M47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2412,15 +2628,13 @@
       <c r="E48" t="s">
         <v>73</v>
       </c>
-      <c r="F48" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I48" t="s">
-        <v>73</v>
-      </c>
-      <c r="J48" t="s">
-        <v>73</v>
-      </c>
+      <c r="F48" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H48" s="3"/>
       <c r="K48" t="s">
         <v>73</v>
       </c>
@@ -2433,8 +2647,14 @@
       <c r="N48" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O48" t="s">
+        <v>73</v>
+      </c>
+      <c r="P48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -2450,13 +2670,13 @@
       <c r="E49" t="s">
         <v>73</v>
       </c>
-      <c r="F49" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I49" t="s">
-        <v>73</v>
-      </c>
-      <c r="J49" t="s">
+      <c r="F49" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H49" s="3" t="s">
         <v>73</v>
       </c>
       <c r="K49" t="s">
@@ -2471,8 +2691,14 @@
       <c r="N49" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O49" t="s">
+        <v>73</v>
+      </c>
+      <c r="P49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2488,18 +2714,18 @@
       <c r="E50" t="s">
         <v>73</v>
       </c>
-      <c r="F50" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H50" t="s">
+      <c r="F50" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J50" t="s">
         <v>106</v>
       </c>
-      <c r="I50" t="s">
-        <v>73</v>
-      </c>
-      <c r="J50" t="s">
-        <v>73</v>
-      </c>
       <c r="K50" t="s">
         <v>73</v>
       </c>
@@ -2512,8 +2738,14 @@
       <c r="N50" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O50" t="s">
+        <v>73</v>
+      </c>
+      <c r="P50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2529,11 +2761,13 @@
       <c r="E51" t="s">
         <v>73</v>
       </c>
-      <c r="H51" t="s">
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="J51" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -2549,11 +2783,13 @@
       <c r="E52" t="s">
         <v>73</v>
       </c>
-      <c r="I52" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="K52" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>27</v>
       </c>
@@ -2569,32 +2805,38 @@
       <c r="E53" t="s">
         <v>97</v>
       </c>
-      <c r="F53" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G53" t="s">
-        <v>73</v>
-      </c>
-      <c r="H53" t="s">
+      <c r="F53" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I53" t="s">
+        <v>73</v>
+      </c>
+      <c r="J53" t="s">
         <v>101</v>
       </c>
-      <c r="I53" t="s">
-        <v>73</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K53" s="2" t="s">
+      <c r="K53" t="s">
+        <v>73</v>
+      </c>
+      <c r="L53" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M53" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N53" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O53" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -2610,8 +2852,10 @@
       <c r="E54" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>32</v>
       </c>
@@ -2627,14 +2871,18 @@
       <c r="E55" t="s">
         <v>73</v>
       </c>
-      <c r="F55" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="J55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F55" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H55" s="3"/>
+      <c r="L55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -2650,8 +2898,10 @@
       <c r="E56" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -2667,8 +2917,10 @@
       <c r="E57" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -2684,32 +2936,38 @@
       <c r="E58" t="s">
         <v>73</v>
       </c>
-      <c r="F58" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G58" t="s">
-        <v>73</v>
-      </c>
-      <c r="H58" t="s">
+      <c r="F58" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I58" t="s">
+        <v>73</v>
+      </c>
+      <c r="J58" t="s">
         <v>102</v>
       </c>
-      <c r="I58" t="s">
-        <v>73</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K58" s="2" t="s">
+      <c r="K58" t="s">
+        <v>73</v>
+      </c>
+      <c r="L58" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M58" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N58" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O58" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P58" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -2725,8 +2983,10 @@
       <c r="E59" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -2742,11 +3002,15 @@
       <c r="E60" t="s">
         <v>73</v>
       </c>
-      <c r="F60" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F60" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H60" s="3"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -2762,11 +3026,15 @@
       <c r="E61" t="s">
         <v>73</v>
       </c>
-      <c r="F61" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F61" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H61" s="3"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -2782,14 +3050,16 @@
       <c r="E62" t="s">
         <v>97</v>
       </c>
-      <c r="G62" t="s">
-        <v>73</v>
-      </c>
-      <c r="H62" t="s">
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" t="s">
+        <v>73</v>
+      </c>
+      <c r="J62" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2805,8 +3075,10 @@
       <c r="E63" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -2822,13 +3094,13 @@
       <c r="E64" t="s">
         <v>73</v>
       </c>
-      <c r="F64" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I64" t="s">
-        <v>73</v>
-      </c>
-      <c r="J64" t="s">
+      <c r="F64" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H64" s="3" t="s">
         <v>73</v>
       </c>
       <c r="K64" t="s">
@@ -2843,8 +3115,14 @@
       <c r="N64" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O64" t="s">
+        <v>73</v>
+      </c>
+      <c r="P64" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -2860,32 +3138,38 @@
       <c r="E65" t="s">
         <v>96</v>
       </c>
-      <c r="F65" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H65" t="s">
+      <c r="F65" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J65" t="s">
         <v>85</v>
       </c>
-      <c r="I65" t="s">
-        <v>73</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K65" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L65" t="s">
+      <c r="K65" t="s">
+        <v>73</v>
+      </c>
+      <c r="L65" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M65" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N65" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N65" t="s">
+        <v>73</v>
+      </c>
+      <c r="O65" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P65" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -2901,29 +3185,35 @@
       <c r="E66" t="s">
         <v>97</v>
       </c>
-      <c r="F66" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G66" t="s">
+      <c r="F66" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H66" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I66" t="s">
         <v>73</v>
       </c>
-      <c r="J66" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K66" s="2" t="s">
+      <c r="K66" t="s">
+        <v>73</v>
+      </c>
+      <c r="L66" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M66" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N66" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O66" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P66" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>21</v>
       </c>
@@ -2939,13 +3229,13 @@
       <c r="E67" t="s">
         <v>73</v>
       </c>
-      <c r="F67" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I67" t="s">
-        <v>73</v>
-      </c>
-      <c r="J67" t="s">
+      <c r="F67" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H67" s="3" t="s">
         <v>73</v>
       </c>
       <c r="K67" t="s">
@@ -2960,9 +3250,15 @@
       <c r="N67" t="s">
         <v>73</v>
       </c>
+      <c r="O67" t="s">
+        <v>73</v>
+      </c>
+      <c r="P67" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N67" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}"/>
+  <autoFilter ref="A1:P67" xr:uid="{8977B742-7604-44F6-A24E-A772E34C6D55}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>